<commit_message>
Added 6/08 moisture data
</commit_message>
<xml_diff>
--- a/moisture.xlsx
+++ b/moisture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiselitrico/Desktop/School related/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiselitrico/Desktop/School related/Dissertation/dissertation-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AB790D0-E15C-824B-9152-A0B7AAEB002A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA012FA-9437-1C49-B18C-C68E2F167CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15240" xr2:uid="{CC85B02B-F75F-F04D-8D32-B60B5D757316}"/>
   </bookViews>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0CB038-4A9D-C24E-804D-548D6346380B}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,13 +442,11 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="D2" s="1">
-        <v>6.05685187</v>
-      </c>
+        <v>47.5</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -459,13 +457,11 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>47.966666666666697</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5.19446092</v>
-      </c>
+        <v>50.2</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -476,13 +472,11 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>53.058333333333302</v>
-      </c>
-      <c r="D4" s="1">
-        <v>4.6097640100000001</v>
-      </c>
+        <v>47.3</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -493,13 +487,11 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>42.358333333333299</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4.5197462399999999</v>
-      </c>
+        <v>51.5</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -510,13 +502,11 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>51.225000000000001</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4.0150002799999998</v>
-      </c>
+        <v>51.3</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -527,13 +517,11 @@
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>52.5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5.5891127899999997</v>
-      </c>
+        <v>53.2</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -544,13 +532,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>42.5416666666667</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4.7046318200000004</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -561,13 +547,11 @@
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>53.5416666666667</v>
-      </c>
-      <c r="D9" s="1">
-        <v>6.8675069400000002</v>
-      </c>
+        <v>55.3</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -578,13 +562,11 @@
         <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>59.183333333333302</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2.8837580699999998</v>
-      </c>
+        <v>54.9</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -595,13 +577,11 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>43.241666666666703</v>
-      </c>
-      <c r="D11" s="1">
-        <v>6.2950858700000003</v>
-      </c>
+        <v>50.8</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -612,13 +592,11 @@
         <v>5</v>
       </c>
       <c r="C12" s="1">
-        <v>52.691666666666698</v>
-      </c>
-      <c r="D12" s="1">
-        <v>8.6660737000000001</v>
-      </c>
+        <v>56.1</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -629,13 +607,11 @@
         <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>60.783333333333402</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2.1263854700000002</v>
-      </c>
+        <v>55.6</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -646,13 +622,11 @@
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>32.766666666666701</v>
-      </c>
-      <c r="D14" s="1">
-        <v>7.4738736899999996</v>
-      </c>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -663,13 +637,11 @@
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>43.008333333333297</v>
-      </c>
-      <c r="D15" s="1">
-        <v>5.0579295699999998</v>
-      </c>
+        <v>45.1</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -680,13 +652,11 @@
         <v>3</v>
       </c>
       <c r="C16" s="1">
-        <v>50.783333333333303</v>
-      </c>
-      <c r="D16" s="1">
-        <v>3.1080052999999999</v>
-      </c>
+        <v>49.3</v>
+      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -697,13 +667,11 @@
         <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>23.316666666666698</v>
-      </c>
-      <c r="D17" s="1">
-        <v>6.4566855199999997</v>
-      </c>
+        <v>38.299999999999997</v>
+      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -714,13 +682,11 @@
         <v>5</v>
       </c>
       <c r="C18" s="1">
-        <v>39.3333333333333</v>
-      </c>
-      <c r="D18" s="1">
-        <v>7.7572644400000001</v>
-      </c>
+        <v>40.4</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -731,13 +697,11 @@
         <v>6</v>
       </c>
       <c r="C19" s="1">
-        <v>49.816666666666698</v>
-      </c>
-      <c r="D19" s="1">
-        <v>5.0233696300000004</v>
-      </c>
+        <v>50.6</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -748,13 +712,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <v>33.625</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="D20" s="1">
-        <v>6.7860987599999998</v>
+        <v>6.05685187</v>
       </c>
       <c r="E20" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -765,13 +729,13 @@
         <v>2</v>
       </c>
       <c r="C21" s="1">
-        <v>44.141666666666701</v>
+        <v>47.966666666666697</v>
       </c>
       <c r="D21" s="1">
-        <v>3.6190049700000002</v>
+        <v>5.19446092</v>
       </c>
       <c r="E21" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -782,13 +746,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="1">
-        <v>53.3</v>
+        <v>53.058333333333302</v>
       </c>
       <c r="D22" s="1">
-        <v>4.3270817399999997</v>
+        <v>4.6097640100000001</v>
       </c>
       <c r="E22" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -799,13 +763,13 @@
         <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>33.558333333333302</v>
+        <v>42.358333333333299</v>
       </c>
       <c r="D23" s="1">
-        <v>5.1508972399999999</v>
+        <v>4.5197462399999999</v>
       </c>
       <c r="E23" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -816,13 +780,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="1">
-        <v>46.783333333333303</v>
+        <v>51.225000000000001</v>
       </c>
       <c r="D24" s="1">
-        <v>5.5815985499999998</v>
+        <v>4.0150002799999998</v>
       </c>
       <c r="E24" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -833,13 +797,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="1">
-        <v>51.65</v>
+        <v>52.5</v>
       </c>
       <c r="D25" s="1">
-        <v>3.5176180000000001</v>
+        <v>5.5891127899999997</v>
       </c>
       <c r="E25" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -850,13 +814,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <v>32.7083333333333</v>
+        <v>42.5416666666667</v>
       </c>
       <c r="D26" s="1">
-        <v>8.3195780399999997</v>
+        <v>4.7046318200000004</v>
       </c>
       <c r="E26" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -867,13 +831,13 @@
         <v>2</v>
       </c>
       <c r="C27" s="1">
-        <v>49.366666666666703</v>
+        <v>53.5416666666667</v>
       </c>
       <c r="D27" s="1">
-        <v>10.204752300000001</v>
+        <v>6.8675069400000002</v>
       </c>
       <c r="E27" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -884,13 +848,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="1">
-        <v>59.391666666666701</v>
+        <v>59.183333333333302</v>
       </c>
       <c r="D28" s="1">
-        <v>3.2351642699999998</v>
+        <v>2.8837580699999998</v>
       </c>
       <c r="E28" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -901,13 +865,13 @@
         <v>4</v>
       </c>
       <c r="C29" s="1">
-        <v>36.35</v>
+        <v>43.241666666666703</v>
       </c>
       <c r="D29" s="1">
-        <v>7.6173844199999996</v>
+        <v>6.2950858700000003</v>
       </c>
       <c r="E29" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -918,13 +882,13 @@
         <v>5</v>
       </c>
       <c r="C30" s="1">
-        <v>48.591666666666697</v>
+        <v>52.691666666666698</v>
       </c>
       <c r="D30" s="1">
-        <v>6.27222714</v>
+        <v>8.6660737000000001</v>
       </c>
       <c r="E30" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -935,13 +899,13 @@
         <v>6</v>
       </c>
       <c r="C31" s="1">
-        <v>59.108333333333299</v>
+        <v>60.783333333333402</v>
       </c>
       <c r="D31" s="1">
-        <v>4.5595969399999996</v>
+        <v>2.1263854700000002</v>
       </c>
       <c r="E31" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -952,13 +916,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>23.816666666666698</v>
+        <v>32.766666666666701</v>
       </c>
       <c r="D32" s="1">
-        <v>7.52907496</v>
+        <v>7.4738736899999996</v>
       </c>
       <c r="E32" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -969,13 +933,13 @@
         <v>2</v>
       </c>
       <c r="C33" s="1">
-        <v>37.591666666666697</v>
+        <v>43.008333333333297</v>
       </c>
       <c r="D33" s="1">
-        <v>5.4809518600000002</v>
+        <v>5.0579295699999998</v>
       </c>
       <c r="E33" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -986,13 +950,13 @@
         <v>3</v>
       </c>
       <c r="C34" s="1">
-        <v>49.875</v>
+        <v>50.783333333333303</v>
       </c>
       <c r="D34" s="1">
-        <v>3.2133598999999999</v>
+        <v>3.1080052999999999</v>
       </c>
       <c r="E34" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1003,13 +967,13 @@
         <v>4</v>
       </c>
       <c r="C35" s="1">
-        <v>16.691666666666698</v>
+        <v>23.316666666666698</v>
       </c>
       <c r="D35" s="1">
-        <v>6.4392910900000002</v>
+        <v>6.4566855199999997</v>
       </c>
       <c r="E35" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1020,13 +984,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="1">
-        <v>33.933333333333302</v>
+        <v>39.3333333333333</v>
       </c>
       <c r="D36" s="1">
-        <v>7.24234183</v>
+        <v>7.7572644400000001</v>
       </c>
       <c r="E36" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1037,13 +1001,13 @@
         <v>6</v>
       </c>
       <c r="C37" s="1">
-        <v>46.266666666666701</v>
+        <v>49.816666666666698</v>
       </c>
       <c r="D37" s="1">
-        <v>5.0517923600000003</v>
+        <v>5.0233696300000004</v>
       </c>
       <c r="E37" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1054,13 +1018,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>30.524999999999999</v>
+        <v>33.625</v>
       </c>
       <c r="D38" s="1">
-        <v>8.0398015600000008</v>
+        <v>6.7860987599999998</v>
       </c>
       <c r="E38" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1071,13 +1035,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="1">
-        <v>39.858333333333299</v>
+        <v>44.141666666666701</v>
       </c>
       <c r="D39" s="1">
-        <v>6.9110528499999999</v>
+        <v>3.6190049700000002</v>
       </c>
       <c r="E39" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1088,13 +1052,13 @@
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>48.95</v>
+        <v>53.3</v>
       </c>
       <c r="D40" s="1">
-        <v>6.43972049</v>
+        <v>4.3270817399999997</v>
       </c>
       <c r="E40" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1105,13 +1069,13 @@
         <v>4</v>
       </c>
       <c r="C41" s="1">
-        <v>27.383333333333301</v>
+        <v>33.558333333333302</v>
       </c>
       <c r="D41" s="1">
-        <v>5.5838783100000002</v>
+        <v>5.1508972399999999</v>
       </c>
       <c r="E41" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1122,13 +1086,13 @@
         <v>5</v>
       </c>
       <c r="C42" s="1">
-        <v>42.274999999999999</v>
+        <v>46.783333333333303</v>
       </c>
       <c r="D42" s="1">
-        <v>7.2376697700000001</v>
+        <v>5.5815985499999998</v>
       </c>
       <c r="E42" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1139,13 +1103,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="1">
-        <v>48.883333333333297</v>
+        <v>51.65</v>
       </c>
       <c r="D43" s="1">
-        <v>4.8771887100000004</v>
+        <v>3.5176180000000001</v>
       </c>
       <c r="E43" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1156,13 +1120,13 @@
         <v>1</v>
       </c>
       <c r="C44" s="1">
-        <v>27.633333333333301</v>
+        <v>32.7083333333333</v>
       </c>
       <c r="D44" s="1">
-        <v>8.6925603900000006</v>
+        <v>8.3195780399999997</v>
       </c>
       <c r="E44" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1173,13 +1137,13 @@
         <v>2</v>
       </c>
       <c r="C45" s="1">
-        <v>42.7</v>
+        <v>49.366666666666703</v>
       </c>
       <c r="D45" s="1">
-        <v>7.64852927</v>
+        <v>10.204752300000001</v>
       </c>
       <c r="E45" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1190,13 +1154,13 @@
         <v>3</v>
       </c>
       <c r="C46" s="1">
-        <v>59.466666666666697</v>
+        <v>59.391666666666701</v>
       </c>
       <c r="D46" s="1">
-        <v>3.30518417</v>
+        <v>3.2351642699999998</v>
       </c>
       <c r="E46" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1207,13 +1171,13 @@
         <v>4</v>
       </c>
       <c r="C47" s="1">
-        <v>29.1666666666667</v>
+        <v>36.35</v>
       </c>
       <c r="D47" s="1">
-        <v>8.2623277999999996</v>
+        <v>7.6173844199999996</v>
       </c>
       <c r="E47" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1224,13 +1188,13 @@
         <v>5</v>
       </c>
       <c r="C48" s="1">
-        <v>44.1666666666667</v>
+        <v>48.591666666666697</v>
       </c>
       <c r="D48" s="1">
-        <v>6.5887415499999999</v>
+        <v>6.27222714</v>
       </c>
       <c r="E48" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1241,13 +1205,13 @@
         <v>6</v>
       </c>
       <c r="C49" s="1">
-        <v>60.741666666666703</v>
+        <v>59.108333333333299</v>
       </c>
       <c r="D49" s="1">
-        <v>2.4126403199999999</v>
+        <v>4.5595969399999996</v>
       </c>
       <c r="E49" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1258,13 +1222,13 @@
         <v>1</v>
       </c>
       <c r="C50" s="1">
-        <v>18.308333333333302</v>
+        <v>23.816666666666698</v>
       </c>
       <c r="D50" s="1">
-        <v>7.15827028</v>
+        <v>7.52907496</v>
       </c>
       <c r="E50" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1275,13 +1239,13 @@
         <v>2</v>
       </c>
       <c r="C51" s="1">
-        <v>33.125</v>
+        <v>37.591666666666697</v>
       </c>
       <c r="D51" s="1">
-        <v>7.6243777699999997</v>
+        <v>5.4809518600000002</v>
       </c>
       <c r="E51" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1292,13 +1256,13 @@
         <v>3</v>
       </c>
       <c r="C52" s="1">
-        <v>48.841666666666697</v>
+        <v>49.875</v>
       </c>
       <c r="D52" s="1">
-        <v>3.23038369</v>
+        <v>3.2133598999999999</v>
       </c>
       <c r="E52" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1309,13 +1273,13 @@
         <v>4</v>
       </c>
       <c r="C53" s="1">
-        <v>13.8166666666667</v>
+        <v>16.691666666666698</v>
       </c>
       <c r="D53" s="1">
-        <v>5.99800472</v>
+        <v>6.4392910900000002</v>
       </c>
       <c r="E53" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1326,13 +1290,13 @@
         <v>5</v>
       </c>
       <c r="C54" s="1">
-        <v>32.0833333333333</v>
+        <v>33.933333333333302</v>
       </c>
       <c r="D54" s="1">
-        <v>8.4126347999999993</v>
+        <v>7.24234183</v>
       </c>
       <c r="E54" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1343,13 +1307,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="1">
-        <v>43.966666666666697</v>
+        <v>46.266666666666701</v>
       </c>
       <c r="D55" s="1">
-        <v>7.2891367899999997</v>
+        <v>5.0517923600000003</v>
       </c>
       <c r="E55" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1360,13 +1324,13 @@
         <v>1</v>
       </c>
       <c r="C56" s="1">
-        <v>22.875</v>
+        <v>30.524999999999999</v>
       </c>
       <c r="D56" s="1">
-        <v>7.0606624699999996</v>
+        <v>8.0398015600000008</v>
       </c>
       <c r="E56" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1377,13 +1341,13 @@
         <v>2</v>
       </c>
       <c r="C57" s="1">
-        <v>33.4</v>
+        <v>39.858333333333299</v>
       </c>
       <c r="D57" s="1">
-        <v>6.6130724499999998</v>
+        <v>6.9110528499999999</v>
       </c>
       <c r="E57" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1394,13 +1358,13 @@
         <v>3</v>
       </c>
       <c r="C58" s="1">
-        <v>45.825000000000003</v>
+        <v>48.95</v>
       </c>
       <c r="D58" s="1">
-        <v>9.1952680499999992</v>
+        <v>6.43972049</v>
       </c>
       <c r="E58" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1411,13 +1375,13 @@
         <v>4</v>
       </c>
       <c r="C59" s="1">
-        <v>19.216666666666701</v>
+        <v>27.383333333333301</v>
       </c>
       <c r="D59" s="1">
-        <v>5.5579318200000003</v>
+        <v>5.5838783100000002</v>
       </c>
       <c r="E59" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1428,13 +1392,13 @@
         <v>5</v>
       </c>
       <c r="C60" s="1">
-        <v>34.325000000000003</v>
+        <v>42.274999999999999</v>
       </c>
       <c r="D60" s="1">
-        <v>6.7669148300000002</v>
+        <v>7.2376697700000001</v>
       </c>
       <c r="E60" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1445,13 +1409,13 @@
         <v>6</v>
       </c>
       <c r="C61" s="1">
-        <v>43.408333333333303</v>
+        <v>48.883333333333297</v>
       </c>
       <c r="D61" s="1">
-        <v>9.05784023</v>
+        <v>4.8771887100000004</v>
       </c>
       <c r="E61" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1462,13 +1426,13 @@
         <v>1</v>
       </c>
       <c r="C62" s="1">
-        <v>16.466666666666701</v>
+        <v>27.633333333333301</v>
       </c>
       <c r="D62" s="1">
-        <v>6.0572020699999998</v>
+        <v>8.6925603900000006</v>
       </c>
       <c r="E62" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1479,13 +1443,13 @@
         <v>2</v>
       </c>
       <c r="C63" s="1">
-        <v>32.616666666666703</v>
+        <v>42.7</v>
       </c>
       <c r="D63" s="1">
-        <v>8.8217534200000003</v>
+        <v>7.64852927</v>
       </c>
       <c r="E63" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -1496,13 +1460,13 @@
         <v>3</v>
       </c>
       <c r="C64" s="1">
-        <v>51.25</v>
+        <v>59.466666666666697</v>
       </c>
       <c r="D64" s="1">
-        <v>4.8451475300000002</v>
+        <v>3.30518417</v>
       </c>
       <c r="E64" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -1513,13 +1477,13 @@
         <v>4</v>
       </c>
       <c r="C65" s="1">
-        <v>16.008333333333301</v>
+        <v>29.1666666666667</v>
       </c>
       <c r="D65" s="1">
-        <v>6.1424688999999999</v>
+        <v>8.2623277999999996</v>
       </c>
       <c r="E65" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -1530,13 +1494,13 @@
         <v>5</v>
       </c>
       <c r="C66" s="1">
-        <v>32.049999999999997</v>
+        <v>44.1666666666667</v>
       </c>
       <c r="D66" s="1">
-        <v>7.7857095200000002</v>
+        <v>6.5887415499999999</v>
       </c>
       <c r="E66" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -1547,13 +1511,13 @@
         <v>6</v>
       </c>
       <c r="C67" s="1">
-        <v>52</v>
+        <v>60.741666666666703</v>
       </c>
       <c r="D67" s="1">
-        <v>3.3709993100000002</v>
+        <v>2.4126403199999999</v>
       </c>
       <c r="E67" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -1564,13 +1528,13 @@
         <v>1</v>
       </c>
       <c r="C68" s="1">
-        <v>11.158333333333299</v>
+        <v>18.308333333333302</v>
       </c>
       <c r="D68" s="1">
-        <v>4.6052259500000003</v>
+        <v>7.15827028</v>
       </c>
       <c r="E68" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -1581,13 +1545,13 @@
         <v>2</v>
       </c>
       <c r="C69" s="1">
-        <v>22.925000000000001</v>
+        <v>33.125</v>
       </c>
       <c r="D69" s="1">
-        <v>6.8871586699999998</v>
+        <v>7.6243777699999997</v>
       </c>
       <c r="E69" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -1598,13 +1562,13 @@
         <v>3</v>
       </c>
       <c r="C70" s="1">
-        <v>42.424999999999997</v>
+        <v>48.841666666666697</v>
       </c>
       <c r="D70" s="1">
-        <v>4.8727675499999998</v>
+        <v>3.23038369</v>
       </c>
       <c r="E70" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -1615,13 +1579,13 @@
         <v>4</v>
       </c>
       <c r="C71" s="1">
-        <v>8.625</v>
+        <v>13.8166666666667</v>
       </c>
       <c r="D71" s="1">
-        <v>2.4521326499999998</v>
+        <v>5.99800472</v>
       </c>
       <c r="E71" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -1632,13 +1596,13 @@
         <v>5</v>
       </c>
       <c r="C72" s="1">
-        <v>23.866666666666699</v>
+        <v>32.0833333333333</v>
       </c>
       <c r="D72" s="1">
-        <v>9.4161692000000006</v>
+        <v>8.4126347999999993</v>
       </c>
       <c r="E72" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -1649,13 +1613,13 @@
         <v>6</v>
       </c>
       <c r="C73" s="1">
-        <v>34.299999999999997</v>
+        <v>43.966666666666697</v>
       </c>
       <c r="D73" s="1">
-        <v>6.2087914199999998</v>
+        <v>7.2891367899999997</v>
       </c>
       <c r="E73" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -1666,13 +1630,13 @@
         <v>1</v>
       </c>
       <c r="C74" s="1">
-        <v>13.4583333333333</v>
+        <v>22.875</v>
       </c>
       <c r="D74" s="1">
-        <v>5.8033624000000001</v>
+        <v>7.0606624699999996</v>
       </c>
       <c r="E74" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -1683,13 +1647,13 @@
         <v>2</v>
       </c>
       <c r="C75" s="1">
-        <v>22.324999999999999</v>
+        <v>33.4</v>
       </c>
       <c r="D75" s="1">
-        <v>6.1614822599999997</v>
+        <v>6.6130724499999998</v>
       </c>
       <c r="E75" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -1700,13 +1664,13 @@
         <v>3</v>
       </c>
       <c r="C76" s="1">
-        <v>36.608333333333299</v>
+        <v>45.825000000000003</v>
       </c>
       <c r="D76" s="1">
-        <v>8.6130406799999992</v>
+        <v>9.1952680499999992</v>
       </c>
       <c r="E76" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -1717,13 +1681,13 @@
         <v>4</v>
       </c>
       <c r="C77" s="1">
-        <v>11.741666666666699</v>
+        <v>19.216666666666701</v>
       </c>
       <c r="D77" s="1">
-        <v>3.84008957</v>
+        <v>5.5579318200000003</v>
       </c>
       <c r="E77" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -1734,13 +1698,13 @@
         <v>5</v>
       </c>
       <c r="C78" s="1">
-        <v>24.875</v>
+        <v>34.325000000000003</v>
       </c>
       <c r="D78" s="1">
-        <v>5.5447149299999996</v>
+        <v>6.7669148300000002</v>
       </c>
       <c r="E78" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -1751,13 +1715,13 @@
         <v>6</v>
       </c>
       <c r="C79" s="1">
-        <v>33.2083333333333</v>
+        <v>43.408333333333303</v>
       </c>
       <c r="D79" s="1">
-        <v>9.7817509400000002</v>
+        <v>9.05784023</v>
       </c>
       <c r="E79" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -1768,13 +1732,13 @@
         <v>1</v>
       </c>
       <c r="C80" s="1">
-        <v>11.366666666666699</v>
+        <v>16.466666666666701</v>
       </c>
       <c r="D80" s="1">
-        <v>4.7105941199999997</v>
+        <v>6.0572020699999998</v>
       </c>
       <c r="E80" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -1785,13 +1749,13 @@
         <v>2</v>
       </c>
       <c r="C81" s="1">
-        <v>20.933333333333302</v>
+        <v>32.616666666666703</v>
       </c>
       <c r="D81" s="1">
-        <v>8.86385237</v>
+        <v>8.8217534200000003</v>
       </c>
       <c r="E81" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -1802,13 +1766,13 @@
         <v>3</v>
       </c>
       <c r="C82" s="1">
-        <v>41.358333333333299</v>
+        <v>51.25</v>
       </c>
       <c r="D82" s="1">
-        <v>5.2184042000000002</v>
+        <v>4.8451475300000002</v>
       </c>
       <c r="E82" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -1819,13 +1783,13 @@
         <v>4</v>
       </c>
       <c r="C83" s="1">
-        <v>9.4</v>
+        <v>16.008333333333301</v>
       </c>
       <c r="D83" s="1">
-        <v>3.5386181200000002</v>
+        <v>6.1424688999999999</v>
       </c>
       <c r="E83" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -1836,13 +1800,13 @@
         <v>5</v>
       </c>
       <c r="C84" s="1">
-        <v>19.074999999999999</v>
+        <v>32.049999999999997</v>
       </c>
       <c r="D84" s="1">
-        <v>6.5026043700000002</v>
+        <v>7.7857095200000002</v>
       </c>
       <c r="E84" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -1853,13 +1817,13 @@
         <v>6</v>
       </c>
       <c r="C85" s="1">
-        <v>39.966666666666697</v>
+        <v>52</v>
       </c>
       <c r="D85" s="1">
-        <v>4.9545816</v>
+        <v>3.3709993100000002</v>
       </c>
       <c r="E85" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -1870,13 +1834,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1">
-        <v>7.4083333333333297</v>
+        <v>11.158333333333299</v>
       </c>
       <c r="D86" s="1">
-        <v>2.47439922</v>
+        <v>4.6052259500000003</v>
       </c>
       <c r="E86" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -1887,13 +1851,13 @@
         <v>2</v>
       </c>
       <c r="C87" s="1">
-        <v>12.383333333333301</v>
+        <v>22.925000000000001</v>
       </c>
       <c r="D87" s="1">
-        <v>4.0260138899999998</v>
+        <v>6.8871586699999998</v>
       </c>
       <c r="E87" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -1904,13 +1868,13 @@
         <v>3</v>
       </c>
       <c r="C88" s="1">
-        <v>29.6</v>
+        <v>42.424999999999997</v>
       </c>
       <c r="D88" s="1">
-        <v>4.42122978</v>
+        <v>4.8727675499999998</v>
       </c>
       <c r="E88" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -1921,13 +1885,13 @@
         <v>4</v>
       </c>
       <c r="C89" s="1">
-        <v>5.9749999999999996</v>
+        <v>8.625</v>
       </c>
       <c r="D89" s="1">
-        <v>2.4391224199999999</v>
+        <v>2.4521326499999998</v>
       </c>
       <c r="E89" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -1938,13 +1902,13 @@
         <v>5</v>
       </c>
       <c r="C90" s="1">
-        <v>14.591666666666701</v>
+        <v>23.866666666666699</v>
       </c>
       <c r="D90" s="1">
-        <v>6.1691989100000004</v>
+        <v>9.4161692000000006</v>
       </c>
       <c r="E90" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -1955,13 +1919,13 @@
         <v>6</v>
       </c>
       <c r="C91" s="1">
-        <v>22.741666666666699</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D91" s="1">
-        <v>5.7722625699999996</v>
+        <v>6.2087914199999998</v>
       </c>
       <c r="E91" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -1972,13 +1936,13 @@
         <v>1</v>
       </c>
       <c r="C92" s="1">
-        <v>11.283333333333299</v>
+        <v>13.4583333333333</v>
       </c>
       <c r="D92" s="1">
-        <v>4.0426888700000001</v>
+        <v>5.8033624000000001</v>
       </c>
       <c r="E92" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -1989,13 +1953,13 @@
         <v>2</v>
       </c>
       <c r="C93" s="1">
-        <v>18.266666666666701</v>
+        <v>22.324999999999999</v>
       </c>
       <c r="D93" s="1">
-        <v>6.4715227000000004</v>
+        <v>6.1614822599999997</v>
       </c>
       <c r="E93" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2006,13 +1970,13 @@
         <v>3</v>
       </c>
       <c r="C94" s="1">
-        <v>28.774999999999999</v>
+        <v>36.608333333333299</v>
       </c>
       <c r="D94" s="1">
-        <v>10.5458415</v>
+        <v>8.6130406799999992</v>
       </c>
       <c r="E94" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2023,13 +1987,13 @@
         <v>4</v>
       </c>
       <c r="C95" s="1">
-        <v>9.0749999999999993</v>
+        <v>11.741666666666699</v>
       </c>
       <c r="D95" s="1">
-        <v>6.5744858099999997</v>
+        <v>3.84008957</v>
       </c>
       <c r="E95" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2040,13 +2004,13 @@
         <v>5</v>
       </c>
       <c r="C96" s="1">
-        <v>21.108333333333299</v>
+        <v>24.875</v>
       </c>
       <c r="D96" s="1">
-        <v>4.77311759</v>
+        <v>5.5447149299999996</v>
       </c>
       <c r="E96" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2057,13 +2021,13 @@
         <v>6</v>
       </c>
       <c r="C97" s="1">
-        <v>28.0833333333333</v>
+        <v>33.2083333333333</v>
       </c>
       <c r="D97" s="1">
-        <v>7.6162306800000001</v>
+        <v>9.7817509400000002</v>
       </c>
       <c r="E97" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -2074,13 +2038,13 @@
         <v>1</v>
       </c>
       <c r="C98" s="1">
-        <v>9.1083333333333307</v>
+        <v>11.366666666666699</v>
       </c>
       <c r="D98" s="1">
-        <v>4.0078237899999998</v>
+        <v>4.7105941199999997</v>
       </c>
       <c r="E98" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -2091,13 +2055,13 @@
         <v>2</v>
       </c>
       <c r="C99" s="1">
-        <v>16.324999999999999</v>
+        <v>20.933333333333302</v>
       </c>
       <c r="D99" s="1">
-        <v>7.5141230700000001</v>
+        <v>8.86385237</v>
       </c>
       <c r="E99" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -2108,13 +2072,13 @@
         <v>3</v>
       </c>
       <c r="C100" s="1">
-        <v>34.391666666666701</v>
+        <v>41.358333333333299</v>
       </c>
       <c r="D100" s="1">
-        <v>7.6958617399999998</v>
+        <v>5.2184042000000002</v>
       </c>
       <c r="E100" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -2125,13 +2089,13 @@
         <v>4</v>
       </c>
       <c r="C101" s="1">
-        <v>7.9166666666666696</v>
+        <v>9.4</v>
       </c>
       <c r="D101" s="1">
-        <v>4.0099497499999996</v>
+        <v>3.5386181200000002</v>
       </c>
       <c r="E101" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -2142,13 +2106,13 @@
         <v>5</v>
       </c>
       <c r="C102" s="1">
-        <v>15.233333333333301</v>
+        <v>19.074999999999999</v>
       </c>
       <c r="D102" s="1">
-        <v>5.2865753399999997</v>
+        <v>6.5026043700000002</v>
       </c>
       <c r="E102" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -2159,13 +2123,13 @@
         <v>6</v>
       </c>
       <c r="C103" s="1">
-        <v>32.7083333333333</v>
+        <v>39.966666666666697</v>
       </c>
       <c r="D103" s="1">
-        <v>10.2219424</v>
+        <v>4.9545816</v>
       </c>
       <c r="E103" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -2176,13 +2140,13 @@
         <v>1</v>
       </c>
       <c r="C104" s="1">
-        <v>5.30833333333333</v>
+        <v>7.4083333333333297</v>
       </c>
       <c r="D104" s="1">
-        <v>1.7095764099999999</v>
+        <v>2.47439922</v>
       </c>
       <c r="E104" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -2193,13 +2157,13 @@
         <v>2</v>
       </c>
       <c r="C105" s="1">
-        <v>9.55833333333333</v>
+        <v>12.383333333333301</v>
       </c>
       <c r="D105" s="1">
-        <v>2.8477928700000001</v>
+        <v>4.0260138899999998</v>
       </c>
       <c r="E105" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -2210,13 +2174,13 @@
         <v>3</v>
       </c>
       <c r="C106" s="1">
-        <v>24.9166666666667</v>
+        <v>29.6</v>
       </c>
       <c r="D106" s="1">
-        <v>6.9137324900000001</v>
+        <v>4.42122978</v>
       </c>
       <c r="E106" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -2227,13 +2191,13 @@
         <v>4</v>
       </c>
       <c r="C107" s="1">
-        <v>5.0333333333333297</v>
+        <v>5.9749999999999996</v>
       </c>
       <c r="D107" s="1">
-        <v>2.2202920900000001</v>
+        <v>2.4391224199999999</v>
       </c>
       <c r="E107" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -2244,13 +2208,13 @@
         <v>5</v>
       </c>
       <c r="C108" s="1">
-        <v>11.1916666666667</v>
+        <v>14.591666666666701</v>
       </c>
       <c r="D108" s="1">
-        <v>3.4431640699999999</v>
+        <v>6.1691989100000004</v>
       </c>
       <c r="E108" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -2261,13 +2225,13 @@
         <v>6</v>
       </c>
       <c r="C109" s="1">
-        <v>16.758333333333301</v>
+        <v>22.741666666666699</v>
       </c>
       <c r="D109" s="1">
-        <v>5.8050852800000001</v>
+        <v>5.7722625699999996</v>
       </c>
       <c r="E109" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -2278,13 +2242,13 @@
         <v>1</v>
       </c>
       <c r="C110" s="1">
-        <v>9.0666666666666593</v>
+        <v>11.283333333333299</v>
       </c>
       <c r="D110" s="1">
-        <v>4.3267315699999997</v>
+        <v>4.0426888700000001</v>
       </c>
       <c r="E110" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -2295,13 +2259,13 @@
         <v>2</v>
       </c>
       <c r="C111" s="1">
-        <v>17.5</v>
+        <v>18.266666666666701</v>
       </c>
       <c r="D111" s="1">
-        <v>6.6420150299999996</v>
+        <v>6.4715227000000004</v>
       </c>
       <c r="E111" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -2312,13 +2276,13 @@
         <v>3</v>
       </c>
       <c r="C112" s="1">
-        <v>33.15</v>
+        <v>28.774999999999999</v>
       </c>
       <c r="D112" s="1">
-        <v>9.6141467699999996</v>
+        <v>10.5458415</v>
       </c>
       <c r="E112" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -2329,13 +2293,13 @@
         <v>4</v>
       </c>
       <c r="C113" s="1">
-        <v>7.3916666666666702</v>
+        <v>9.0749999999999993</v>
       </c>
       <c r="D113" s="1">
-        <v>4.1491419299999999</v>
+        <v>6.5744858099999997</v>
       </c>
       <c r="E113" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -2346,13 +2310,13 @@
         <v>5</v>
       </c>
       <c r="C114" s="1">
-        <v>18.2916666666667</v>
+        <v>21.108333333333299</v>
       </c>
       <c r="D114" s="1">
-        <v>5.3595214100000002</v>
+        <v>4.77311759</v>
       </c>
       <c r="E114" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -2363,13 +2327,13 @@
         <v>6</v>
       </c>
       <c r="C115" s="1">
-        <v>25.983333333333299</v>
+        <v>28.0833333333333</v>
       </c>
       <c r="D115" s="1">
-        <v>8.5988195100000002</v>
+        <v>7.6162306800000001</v>
       </c>
       <c r="E115" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -2380,13 +2344,13 @@
         <v>1</v>
       </c>
       <c r="C116" s="1">
-        <v>9.0166666666666693</v>
+        <v>9.1083333333333307</v>
       </c>
       <c r="D116" s="1">
-        <v>3.0234938599999999</v>
+        <v>4.0078237899999998</v>
       </c>
       <c r="E116" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -2397,13 +2361,13 @@
         <v>2</v>
       </c>
       <c r="C117" s="1">
-        <v>14.6916666666667</v>
+        <v>16.324999999999999</v>
       </c>
       <c r="D117" s="1">
-        <v>5.5299939699999996</v>
+        <v>7.5141230700000001</v>
       </c>
       <c r="E117" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -2414,13 +2378,13 @@
         <v>3</v>
       </c>
       <c r="C118" s="1">
-        <v>33.725000000000001</v>
+        <v>34.391666666666701</v>
       </c>
       <c r="D118" s="1">
-        <v>10.120287899999999</v>
+        <v>7.6958617399999998</v>
       </c>
       <c r="E118" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -2431,13 +2395,13 @@
         <v>4</v>
       </c>
       <c r="C119" s="1">
-        <v>8.4916666666666707</v>
+        <v>7.9166666666666696</v>
       </c>
       <c r="D119" s="1">
-        <v>4.81559179</v>
+        <v>4.0099497499999996</v>
       </c>
       <c r="E119" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -2448,13 +2412,13 @@
         <v>5</v>
       </c>
       <c r="C120" s="1">
-        <v>13.225</v>
+        <v>15.233333333333301</v>
       </c>
       <c r="D120" s="1">
-        <v>4.6331071499999998</v>
+        <v>5.2865753399999997</v>
       </c>
       <c r="E120" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -2465,13 +2429,13 @@
         <v>6</v>
       </c>
       <c r="C121" s="1">
-        <v>30.941666666666698</v>
+        <v>32.7083333333333</v>
       </c>
       <c r="D121" s="1">
-        <v>12.5605051</v>
+        <v>10.2219424</v>
       </c>
       <c r="E121" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -2482,13 +2446,13 @@
         <v>1</v>
       </c>
       <c r="C122" s="1">
-        <v>5.4666666666666703</v>
+        <v>5.30833333333333</v>
       </c>
       <c r="D122" s="1">
-        <v>2.6776289800000002</v>
+        <v>1.7095764099999999</v>
       </c>
       <c r="E122" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -2499,13 +2463,13 @@
         <v>2</v>
       </c>
       <c r="C123" s="1">
-        <v>8.9083333333333297</v>
+        <v>9.55833333333333</v>
       </c>
       <c r="D123" s="1">
-        <v>3.2814792499999998</v>
+        <v>2.8477928700000001</v>
       </c>
       <c r="E123" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -2516,13 +2480,13 @@
         <v>3</v>
       </c>
       <c r="C124" s="1">
-        <v>21.975000000000001</v>
+        <v>24.9166666666667</v>
       </c>
       <c r="D124" s="1">
-        <v>9.1335669599999996</v>
+        <v>6.9137324900000001</v>
       </c>
       <c r="E124" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -2533,13 +2497,13 @@
         <v>4</v>
       </c>
       <c r="C125" s="1">
-        <v>6.0916666666666703</v>
+        <v>5.0333333333333297</v>
       </c>
       <c r="D125" s="1">
-        <v>2.81633493</v>
+        <v>2.2202920900000001</v>
       </c>
       <c r="E125" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -2550,13 +2514,13 @@
         <v>5</v>
       </c>
       <c r="C126" s="1">
-        <v>9.2750000000000004</v>
+        <v>11.1916666666667</v>
       </c>
       <c r="D126" s="1">
-        <v>3.4892367000000002</v>
+        <v>3.4431640699999999</v>
       </c>
       <c r="E126" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -2567,12 +2531,318 @@
         <v>6</v>
       </c>
       <c r="C127" s="1">
+        <v>16.758333333333301</v>
+      </c>
+      <c r="D127" s="1">
+        <v>5.8050852800000001</v>
+      </c>
+      <c r="E127" s="2">
+        <v>44793</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+      <c r="C128" s="1">
+        <v>9.0666666666666593</v>
+      </c>
+      <c r="D128" s="1">
+        <v>4.3267315699999997</v>
+      </c>
+      <c r="E128" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <v>2</v>
+      </c>
+      <c r="C129" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="D129" s="1">
+        <v>6.6420150299999996</v>
+      </c>
+      <c r="E129" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1</v>
+      </c>
+      <c r="B130">
+        <v>3</v>
+      </c>
+      <c r="C130" s="1">
+        <v>33.15</v>
+      </c>
+      <c r="D130" s="1">
+        <v>9.6141467699999996</v>
+      </c>
+      <c r="E130" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>4</v>
+      </c>
+      <c r="C131" s="1">
+        <v>7.3916666666666702</v>
+      </c>
+      <c r="D131" s="1">
+        <v>4.1491419299999999</v>
+      </c>
+      <c r="E131" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1</v>
+      </c>
+      <c r="B132">
+        <v>5</v>
+      </c>
+      <c r="C132" s="1">
+        <v>18.2916666666667</v>
+      </c>
+      <c r="D132" s="1">
+        <v>5.3595214100000002</v>
+      </c>
+      <c r="E132" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133">
+        <v>6</v>
+      </c>
+      <c r="C133" s="1">
+        <v>25.983333333333299</v>
+      </c>
+      <c r="D133" s="1">
+        <v>8.5988195100000002</v>
+      </c>
+      <c r="E133" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>2</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134" s="1">
+        <v>9.0166666666666693</v>
+      </c>
+      <c r="D134" s="1">
+        <v>3.0234938599999999</v>
+      </c>
+      <c r="E134" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>2</v>
+      </c>
+      <c r="B135">
+        <v>2</v>
+      </c>
+      <c r="C135" s="1">
+        <v>14.6916666666667</v>
+      </c>
+      <c r="D135" s="1">
+        <v>5.5299939699999996</v>
+      </c>
+      <c r="E135" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>2</v>
+      </c>
+      <c r="B136">
+        <v>3</v>
+      </c>
+      <c r="C136" s="1">
+        <v>33.725000000000001</v>
+      </c>
+      <c r="D136" s="1">
+        <v>10.120287899999999</v>
+      </c>
+      <c r="E136" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>2</v>
+      </c>
+      <c r="B137">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1">
+        <v>8.4916666666666707</v>
+      </c>
+      <c r="D137" s="1">
+        <v>4.81559179</v>
+      </c>
+      <c r="E137" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>2</v>
+      </c>
+      <c r="B138">
+        <v>5</v>
+      </c>
+      <c r="C138" s="1">
+        <v>13.225</v>
+      </c>
+      <c r="D138" s="1">
+        <v>4.6331071499999998</v>
+      </c>
+      <c r="E138" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>2</v>
+      </c>
+      <c r="B139">
+        <v>6</v>
+      </c>
+      <c r="C139" s="1">
+        <v>30.941666666666698</v>
+      </c>
+      <c r="D139" s="1">
+        <v>12.5605051</v>
+      </c>
+      <c r="E139" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>3</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+      <c r="C140" s="1">
+        <v>5.4666666666666703</v>
+      </c>
+      <c r="D140" s="1">
+        <v>2.6776289800000002</v>
+      </c>
+      <c r="E140" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>3</v>
+      </c>
+      <c r="B141">
+        <v>2</v>
+      </c>
+      <c r="C141" s="1">
+        <v>8.9083333333333297</v>
+      </c>
+      <c r="D141" s="1">
+        <v>3.2814792499999998</v>
+      </c>
+      <c r="E141" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>3</v>
+      </c>
+      <c r="B142">
+        <v>3</v>
+      </c>
+      <c r="C142" s="1">
+        <v>21.975000000000001</v>
+      </c>
+      <c r="D142" s="1">
+        <v>9.1335669599999996</v>
+      </c>
+      <c r="E142" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>3</v>
+      </c>
+      <c r="B143">
+        <v>4</v>
+      </c>
+      <c r="C143" s="1">
+        <v>6.0916666666666703</v>
+      </c>
+      <c r="D143" s="1">
+        <v>2.81633493</v>
+      </c>
+      <c r="E143" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>3</v>
+      </c>
+      <c r="B144">
+        <v>5</v>
+      </c>
+      <c r="C144" s="1">
+        <v>9.2750000000000004</v>
+      </c>
+      <c r="D144" s="1">
+        <v>3.4892367000000002</v>
+      </c>
+      <c r="E144" s="2">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>3</v>
+      </c>
+      <c r="B145">
+        <v>6</v>
+      </c>
+      <c r="C145" s="1">
         <v>14.783333333333299</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D145" s="1">
         <v>7.5559529000000003</v>
       </c>
-      <c r="E127" s="2">
+      <c r="E145" s="2">
         <v>44796</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added water volume irrigation data
</commit_message>
<xml_diff>
--- a/moisture.xlsx
+++ b/moisture.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiselitrico/Desktop/School related/Dissertation/dissertation-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA012FA-9437-1C49-B18C-C68E2F167CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476F49FD-08CB-FC41-B55D-ED27FB414F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15240" xr2:uid="{CC85B02B-F75F-F04D-8D32-B60B5D757316}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>date</t>
   </si>
@@ -49,6 +50,9 @@
   </si>
   <si>
     <t>soil_type</t>
+  </si>
+  <si>
+    <t>irrigation</t>
   </si>
 </sst>
 </file>
@@ -409,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0CB038-4A9D-C24E-804D-548D6346380B}">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -433,8 +437,11 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -448,8 +455,11 @@
       <c r="E2" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -463,8 +473,11 @@
       <c r="E3" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -478,8 +491,11 @@
       <c r="E4" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -493,8 +509,11 @@
       <c r="E5" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -508,8 +527,11 @@
       <c r="E6" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -523,8 +545,11 @@
       <c r="E7" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -538,8 +563,11 @@
       <c r="E8" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -553,8 +581,11 @@
       <c r="E9" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -568,8 +599,11 @@
       <c r="E10" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -583,8 +617,11 @@
       <c r="E11" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -598,8 +635,11 @@
       <c r="E12" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -613,8 +653,11 @@
       <c r="E13" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -628,8 +671,11 @@
       <c r="E14" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -643,8 +689,11 @@
       <c r="E15" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -658,8 +707,11 @@
       <c r="E16" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -673,8 +725,11 @@
       <c r="E17" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -688,8 +743,11 @@
       <c r="E18" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -703,8 +761,11 @@
       <c r="E19" s="2">
         <v>44779</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -720,8 +781,11 @@
       <c r="E20" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -737,8 +801,11 @@
       <c r="E21" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -754,8 +821,11 @@
       <c r="E22" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -771,8 +841,11 @@
       <c r="E23" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -788,8 +861,11 @@
       <c r="E24" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -805,8 +881,11 @@
       <c r="E25" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -822,8 +901,11 @@
       <c r="E26" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -839,8 +921,11 @@
       <c r="E27" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -856,8 +941,11 @@
       <c r="E28" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -873,8 +961,11 @@
       <c r="E29" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -890,8 +981,11 @@
       <c r="E30" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -907,8 +1001,11 @@
       <c r="E31" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -924,8 +1021,11 @@
       <c r="E32" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -941,8 +1041,11 @@
       <c r="E33" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -958,8 +1061,11 @@
       <c r="E34" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -975,8 +1081,11 @@
       <c r="E35" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -992,8 +1101,11 @@
       <c r="E36" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1009,8 +1121,11 @@
       <c r="E37" s="2">
         <v>44782</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1026,8 +1141,11 @@
       <c r="E38" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1043,8 +1161,11 @@
       <c r="E39" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1060,8 +1181,11 @@
       <c r="E40" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1077,8 +1201,11 @@
       <c r="E41" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1094,8 +1221,11 @@
       <c r="E42" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1111,8 +1241,11 @@
       <c r="E43" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1128,8 +1261,11 @@
       <c r="E44" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1145,8 +1281,11 @@
       <c r="E45" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1162,8 +1301,11 @@
       <c r="E46" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1179,8 +1321,11 @@
       <c r="E47" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1196,8 +1341,11 @@
       <c r="E48" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1213,8 +1361,11 @@
       <c r="E49" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1230,8 +1381,11 @@
       <c r="E50" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -1247,8 +1401,11 @@
       <c r="E51" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -1264,8 +1421,11 @@
       <c r="E52" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -1281,8 +1441,11 @@
       <c r="E53" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -1298,8 +1461,11 @@
       <c r="E54" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3</v>
       </c>
@@ -1315,8 +1481,11 @@
       <c r="E55" s="2">
         <v>44784</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1332,8 +1501,11 @@
       <c r="E56" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -1349,8 +1521,11 @@
       <c r="E57" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1366,8 +1541,11 @@
       <c r="E58" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1383,8 +1561,11 @@
       <c r="E59" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1400,8 +1581,11 @@
       <c r="E60" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -1417,8 +1601,11 @@
       <c r="E61" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
@@ -1434,8 +1621,11 @@
       <c r="E62" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
@@ -1451,8 +1641,11 @@
       <c r="E63" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -1468,8 +1661,11 @@
       <c r="E64" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
@@ -1485,8 +1681,11 @@
       <c r="E65" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
@@ -1502,8 +1701,11 @@
       <c r="E66" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
@@ -1519,8 +1721,11 @@
       <c r="E67" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>3</v>
       </c>
@@ -1536,8 +1741,11 @@
       <c r="E68" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>3</v>
       </c>
@@ -1553,8 +1761,11 @@
       <c r="E69" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>3</v>
       </c>
@@ -1570,8 +1781,11 @@
       <c r="E70" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>3</v>
       </c>
@@ -1587,8 +1801,11 @@
       <c r="E71" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>3</v>
       </c>
@@ -1604,8 +1821,11 @@
       <c r="E72" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>3</v>
       </c>
@@ -1621,8 +1841,11 @@
       <c r="E73" s="2">
         <v>44786</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -1638,8 +1861,11 @@
       <c r="E74" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1655,8 +1881,11 @@
       <c r="E75" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1</v>
       </c>
@@ -1672,8 +1901,11 @@
       <c r="E76" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1</v>
       </c>
@@ -1689,8 +1921,11 @@
       <c r="E77" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1</v>
       </c>
@@ -1706,8 +1941,11 @@
       <c r="E78" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1</v>
       </c>
@@ -1723,8 +1961,11 @@
       <c r="E79" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2</v>
       </c>
@@ -1740,8 +1981,11 @@
       <c r="E80" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2</v>
       </c>
@@ -1757,8 +2001,11 @@
       <c r="E81" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2</v>
       </c>
@@ -1774,8 +2021,11 @@
       <c r="E82" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2</v>
       </c>
@@ -1791,8 +2041,11 @@
       <c r="E83" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2</v>
       </c>
@@ -1808,8 +2061,11 @@
       <c r="E84" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2</v>
       </c>
@@ -1825,8 +2081,11 @@
       <c r="E85" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>3</v>
       </c>
@@ -1842,8 +2101,11 @@
       <c r="E86" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>3</v>
       </c>
@@ -1859,8 +2121,11 @@
       <c r="E87" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>3</v>
       </c>
@@ -1876,8 +2141,11 @@
       <c r="E88" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>3</v>
       </c>
@@ -1893,8 +2161,11 @@
       <c r="E89" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>3</v>
       </c>
@@ -1910,8 +2181,11 @@
       <c r="E90" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>3</v>
       </c>
@@ -1927,8 +2201,11 @@
       <c r="E91" s="2">
         <v>44789</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -1944,8 +2221,11 @@
       <c r="E92" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -1961,8 +2241,11 @@
       <c r="E93" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
@@ -1978,8 +2261,11 @@
       <c r="E94" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1</v>
       </c>
@@ -1995,8 +2281,11 @@
       <c r="E95" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1</v>
       </c>
@@ -2012,8 +2301,11 @@
       <c r="E96" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1</v>
       </c>
@@ -2029,8 +2321,11 @@
       <c r="E97" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2</v>
       </c>
@@ -2046,8 +2341,11 @@
       <c r="E98" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2</v>
       </c>
@@ -2063,8 +2361,11 @@
       <c r="E99" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2</v>
       </c>
@@ -2080,8 +2381,11 @@
       <c r="E100" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2</v>
       </c>
@@ -2097,8 +2401,11 @@
       <c r="E101" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2</v>
       </c>
@@ -2114,8 +2421,11 @@
       <c r="E102" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2</v>
       </c>
@@ -2131,8 +2441,11 @@
       <c r="E103" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>3</v>
       </c>
@@ -2148,8 +2461,11 @@
       <c r="E104" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>3</v>
       </c>
@@ -2165,8 +2481,11 @@
       <c r="E105" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>3</v>
       </c>
@@ -2182,8 +2501,11 @@
       <c r="E106" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>3</v>
       </c>
@@ -2199,8 +2521,11 @@
       <c r="E107" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>3</v>
       </c>
@@ -2216,8 +2541,11 @@
       <c r="E108" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>3</v>
       </c>
@@ -2233,8 +2561,11 @@
       <c r="E109" s="2">
         <v>44791</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1</v>
       </c>
@@ -2250,8 +2581,11 @@
       <c r="E110" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>1</v>
       </c>
@@ -2267,8 +2601,11 @@
       <c r="E111" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1</v>
       </c>
@@ -2284,8 +2621,11 @@
       <c r="E112" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>1</v>
       </c>
@@ -2301,8 +2641,11 @@
       <c r="E113" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1</v>
       </c>
@@ -2318,8 +2661,11 @@
       <c r="E114" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>1</v>
       </c>
@@ -2335,8 +2681,11 @@
       <c r="E115" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2</v>
       </c>
@@ -2352,8 +2701,11 @@
       <c r="E116" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2</v>
       </c>
@@ -2369,8 +2721,11 @@
       <c r="E117" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2</v>
       </c>
@@ -2386,8 +2741,11 @@
       <c r="E118" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2</v>
       </c>
@@ -2403,8 +2761,11 @@
       <c r="E119" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2</v>
       </c>
@@ -2420,8 +2781,11 @@
       <c r="E120" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2</v>
       </c>
@@ -2437,8 +2801,11 @@
       <c r="E121" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>3</v>
       </c>
@@ -2454,8 +2821,11 @@
       <c r="E122" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>3</v>
       </c>
@@ -2471,8 +2841,11 @@
       <c r="E123" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>3</v>
       </c>
@@ -2488,8 +2861,11 @@
       <c r="E124" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>3</v>
       </c>
@@ -2505,8 +2881,11 @@
       <c r="E125" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>3</v>
       </c>
@@ -2522,8 +2901,11 @@
       <c r="E126" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>3</v>
       </c>
@@ -2539,8 +2921,11 @@
       <c r="E127" s="2">
         <v>44793</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F127">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>1</v>
       </c>
@@ -2556,8 +2941,11 @@
       <c r="E128" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1</v>
       </c>
@@ -2573,8 +2961,11 @@
       <c r="E129" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1</v>
       </c>
@@ -2590,8 +2981,11 @@
       <c r="E130" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>1</v>
       </c>
@@ -2607,8 +3001,11 @@
       <c r="E131" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1</v>
       </c>
@@ -2624,8 +3021,11 @@
       <c r="E132" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1</v>
       </c>
@@ -2641,8 +3041,11 @@
       <c r="E133" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>2</v>
       </c>
@@ -2658,8 +3061,11 @@
       <c r="E134" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2</v>
       </c>
@@ -2675,8 +3081,11 @@
       <c r="E135" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2</v>
       </c>
@@ -2692,8 +3101,11 @@
       <c r="E136" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2</v>
       </c>
@@ -2709,8 +3121,11 @@
       <c r="E137" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2</v>
       </c>
@@ -2726,8 +3141,11 @@
       <c r="E138" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2</v>
       </c>
@@ -2743,8 +3161,11 @@
       <c r="E139" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>3</v>
       </c>
@@ -2760,8 +3181,11 @@
       <c r="E140" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>3</v>
       </c>
@@ -2777,8 +3201,11 @@
       <c r="E141" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>3</v>
       </c>
@@ -2794,8 +3221,11 @@
       <c r="E142" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>3</v>
       </c>
@@ -2811,8 +3241,11 @@
       <c r="E143" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>3</v>
       </c>
@@ -2828,8 +3261,11 @@
       <c r="E144" s="2">
         <v>44796</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>3</v>
       </c>
@@ -2844,6 +3280,9 @@
       </c>
       <c r="E145" s="2">
         <v>44796</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed irrigation measures for last day according to notebook
</commit_message>
<xml_diff>
--- a/moisture.xlsx
+++ b/moisture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiselitrico/Desktop/School related/Dissertation/dissertation-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8D9772-97D2-5444-8123-9702D8F5346B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5AB89B-6564-934D-9779-42CE2B46D348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15240" xr2:uid="{CC85B02B-F75F-F04D-8D32-B60B5D757316}"/>
   </bookViews>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0CB038-4A9D-C24E-804D-548D6346380B}">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="L117" sqref="L117"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="J135" sqref="J135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3326,7 +3326,7 @@
         <v>44796</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G128">
         <v>248</v>
@@ -3349,7 +3349,7 @@
         <v>44796</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G129">
         <v>325</v>
@@ -3372,7 +3372,7 @@
         <v>44796</v>
       </c>
       <c r="F130">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G130">
         <v>405</v>
@@ -3395,7 +3395,7 @@
         <v>44796</v>
       </c>
       <c r="F131">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G131">
         <v>242</v>
@@ -3418,7 +3418,7 @@
         <v>44796</v>
       </c>
       <c r="F132">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G132">
         <v>315</v>
@@ -3441,7 +3441,7 @@
         <v>44796</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G133">
         <v>375</v>
@@ -3464,7 +3464,7 @@
         <v>44796</v>
       </c>
       <c r="F134">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G134">
         <v>260</v>
@@ -3487,7 +3487,7 @@
         <v>44796</v>
       </c>
       <c r="F135">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G135">
         <v>325</v>
@@ -3510,7 +3510,7 @@
         <v>44796</v>
       </c>
       <c r="F136">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G136">
         <v>415</v>
@@ -3533,7 +3533,7 @@
         <v>44796</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G137">
         <v>240</v>
@@ -3556,7 +3556,7 @@
         <v>44796</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G138">
         <v>312</v>
@@ -3579,7 +3579,7 @@
         <v>44796</v>
       </c>
       <c r="F139">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G139">
         <v>420</v>
@@ -3602,7 +3602,7 @@
         <v>44796</v>
       </c>
       <c r="F140">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G140">
         <v>472</v>
@@ -3625,7 +3625,7 @@
         <v>44796</v>
       </c>
       <c r="F141">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G141">
         <v>498</v>
@@ -3648,7 +3648,7 @@
         <v>44796</v>
       </c>
       <c r="F142">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G142">
         <v>580</v>
@@ -3671,7 +3671,7 @@
         <v>44796</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G143">
         <v>455</v>
@@ -3694,7 +3694,7 @@
         <v>44796</v>
       </c>
       <c r="F144">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G144">
         <v>530</v>
@@ -3717,7 +3717,7 @@
         <v>44796</v>
       </c>
       <c r="F145">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G145">
         <v>591</v>

</xml_diff>

<commit_message>
added day 4/08 + changed graphs accordingly
</commit_message>
<xml_diff>
--- a/moisture.xlsx
+++ b/moisture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louiselitrico/Desktop/School related/Dissertation/dissertation-work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5AB89B-6564-934D-9779-42CE2B46D348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2954C6-B655-FC40-BFE7-3490F8859D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15240" xr2:uid="{CC85B02B-F75F-F04D-8D32-B60B5D757316}"/>
   </bookViews>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0CB038-4A9D-C24E-804D-548D6346380B}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="J135" sqref="J135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,18 +454,16 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>47.5</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F2">
         <v>60</v>
       </c>
       <c r="G2">
-        <v>590</v>
+        <v>755</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -475,18 +473,16 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>50.2</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F3">
         <v>90</v>
       </c>
       <c r="G3">
-        <v>550</v>
+        <v>750</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -496,18 +492,16 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>47.3</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F4">
         <v>120</v>
       </c>
       <c r="G4">
-        <v>510</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -517,18 +511,16 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>51.5</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F5">
         <v>60</v>
       </c>
       <c r="G5">
-        <v>525</v>
+        <v>800</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -538,18 +530,16 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
-        <v>51.3</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F6">
         <v>90</v>
       </c>
       <c r="G6">
-        <v>520</v>
+        <v>750</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -559,18 +549,16 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
-        <v>53.2</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F7">
         <v>120</v>
       </c>
       <c r="G7">
-        <v>540</v>
+        <v>850</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -580,18 +568,16 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>49</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F8">
         <v>60</v>
       </c>
       <c r="G8">
-        <v>540</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -601,18 +587,16 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="1">
-        <v>55.3</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F9">
         <v>90</v>
       </c>
       <c r="G9">
-        <v>590</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -622,18 +606,16 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>54.9</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F10">
         <v>120</v>
       </c>
       <c r="G10">
-        <v>555</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -643,18 +625,16 @@
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="C11" s="1">
-        <v>50.8</v>
-      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F11">
         <v>60</v>
       </c>
       <c r="G11">
-        <v>540</v>
+        <v>600</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -664,18 +644,16 @@
       <c r="B12">
         <v>5</v>
       </c>
-      <c r="C12" s="1">
-        <v>56.1</v>
-      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F12">
         <v>90</v>
       </c>
       <c r="G12">
-        <v>590</v>
+        <v>625</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -685,18 +663,16 @@
       <c r="B13">
         <v>6</v>
       </c>
-      <c r="C13" s="1">
-        <v>55.6</v>
-      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F13">
         <v>120</v>
       </c>
       <c r="G13">
-        <v>590</v>
+        <v>605</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -706,18 +682,16 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
-        <v>39.799999999999997</v>
-      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F14">
         <v>60</v>
       </c>
       <c r="G14">
-        <v>690</v>
+        <v>552</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -727,18 +701,16 @@
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="1">
-        <v>45.1</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F15">
         <v>90</v>
       </c>
       <c r="G15">
-        <v>725</v>
+        <v>590</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -748,18 +720,16 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" s="1">
-        <v>49.3</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F16">
         <v>120</v>
       </c>
       <c r="G16">
-        <v>730</v>
+        <v>545</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -769,18 +739,16 @@
       <c r="B17">
         <v>4</v>
       </c>
-      <c r="C17" s="1">
-        <v>38.299999999999997</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F17">
         <v>60</v>
       </c>
       <c r="G17">
-        <v>720</v>
+        <v>590</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -790,18 +758,16 @@
       <c r="B18">
         <v>5</v>
       </c>
-      <c r="C18" s="1">
-        <v>40.4</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F18">
         <v>90</v>
       </c>
       <c r="G18">
-        <v>730</v>
+        <v>550</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -811,18 +777,16 @@
       <c r="B19">
         <v>6</v>
       </c>
-      <c r="C19" s="1">
-        <v>50.6</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="2">
-        <v>44779</v>
+        <v>44777</v>
       </c>
       <c r="F19">
         <v>120</v>
       </c>
       <c r="G19">
-        <v>825</v>
+        <v>570</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -833,19 +797,17 @@
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="D20" s="1">
-        <v>6.05685187</v>
-      </c>
+        <v>47.5</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F20">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G20">
-        <v>455</v>
+        <v>590</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -856,19 +818,17 @@
         <v>2</v>
       </c>
       <c r="C21" s="1">
-        <v>47.966666666666697</v>
-      </c>
-      <c r="D21" s="1">
-        <v>5.19446092</v>
-      </c>
+        <v>50.2</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F21">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G21">
-        <v>530</v>
+        <v>550</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -879,19 +839,17 @@
         <v>3</v>
       </c>
       <c r="C22" s="1">
-        <v>53.058333333333302</v>
-      </c>
-      <c r="D22" s="1">
-        <v>4.6097640100000001</v>
-      </c>
+        <v>47.3</v>
+      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F22">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G22">
-        <v>520</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -902,19 +860,17 @@
         <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>42.358333333333299</v>
-      </c>
-      <c r="D23" s="1">
-        <v>4.5197462399999999</v>
-      </c>
+        <v>51.5</v>
+      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F23">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G23">
-        <v>480</v>
+        <v>525</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -925,19 +881,17 @@
         <v>5</v>
       </c>
       <c r="C24" s="1">
-        <v>51.225000000000001</v>
-      </c>
-      <c r="D24" s="1">
-        <v>4.0150002799999998</v>
-      </c>
+        <v>51.3</v>
+      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F24">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G24">
-        <v>515</v>
+        <v>520</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -948,19 +902,17 @@
         <v>6</v>
       </c>
       <c r="C25" s="1">
-        <v>52.5</v>
-      </c>
-      <c r="D25" s="1">
-        <v>5.5891127899999997</v>
-      </c>
+        <v>53.2</v>
+      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G25">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -971,19 +923,17 @@
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <v>42.5416666666667</v>
-      </c>
-      <c r="D26" s="1">
-        <v>4.7046318200000004</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F26">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G26">
-        <v>520</v>
+        <v>540</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -994,19 +944,17 @@
         <v>2</v>
       </c>
       <c r="C27" s="1">
-        <v>53.5416666666667</v>
-      </c>
-      <c r="D27" s="1">
-        <v>6.8675069400000002</v>
-      </c>
+        <v>55.3</v>
+      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F27">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G27">
-        <v>570</v>
+        <v>590</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1017,19 +965,17 @@
         <v>3</v>
       </c>
       <c r="C28" s="1">
-        <v>59.183333333333302</v>
-      </c>
-      <c r="D28" s="1">
-        <v>2.8837580699999998</v>
-      </c>
+        <v>54.9</v>
+      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F28">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G28">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1040,19 +986,17 @@
         <v>4</v>
       </c>
       <c r="C29" s="1">
-        <v>43.241666666666703</v>
-      </c>
-      <c r="D29" s="1">
-        <v>6.2950858700000003</v>
-      </c>
+        <v>50.8</v>
+      </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F29">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G29">
-        <v>490</v>
+        <v>540</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1063,19 +1007,17 @@
         <v>5</v>
       </c>
       <c r="C30" s="1">
-        <v>52.691666666666698</v>
-      </c>
-      <c r="D30" s="1">
-        <v>8.6660737000000001</v>
-      </c>
+        <v>56.1</v>
+      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F30">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G30">
-        <v>570</v>
+        <v>590</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1086,19 +1028,17 @@
         <v>6</v>
       </c>
       <c r="C31" s="1">
-        <v>60.783333333333402</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2.1263854700000002</v>
-      </c>
+        <v>55.6</v>
+      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F31">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G31">
-        <v>600</v>
+        <v>590</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1109,19 +1049,17 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>32.766666666666701</v>
-      </c>
-      <c r="D32" s="1">
-        <v>7.4738736899999996</v>
-      </c>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F32">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G32">
-        <v>645</v>
+        <v>690</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1132,19 +1070,17 @@
         <v>2</v>
       </c>
       <c r="C33" s="1">
-        <v>43.008333333333297</v>
-      </c>
-      <c r="D33" s="1">
-        <v>5.0579295699999998</v>
-      </c>
+        <v>45.1</v>
+      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F33">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G33">
-        <v>710</v>
+        <v>725</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1155,16 +1091,14 @@
         <v>3</v>
       </c>
       <c r="C34" s="1">
-        <v>50.783333333333303</v>
-      </c>
-      <c r="D34" s="1">
-        <v>3.1080052999999999</v>
-      </c>
+        <v>49.3</v>
+      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F34">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G34">
         <v>730</v>
@@ -1178,19 +1112,17 @@
         <v>4</v>
       </c>
       <c r="C35" s="1">
-        <v>23.316666666666698</v>
-      </c>
-      <c r="D35" s="1">
-        <v>6.4566855199999997</v>
-      </c>
+        <v>38.299999999999997</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F35">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G35">
-        <v>625</v>
+        <v>720</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1201,19 +1133,17 @@
         <v>5</v>
       </c>
       <c r="C36" s="1">
-        <v>39.3333333333333</v>
-      </c>
-      <c r="D36" s="1">
-        <v>7.7572644400000001</v>
-      </c>
+        <v>40.4</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F36">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G36">
-        <v>720</v>
+        <v>730</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1224,19 +1154,17 @@
         <v>6</v>
       </c>
       <c r="C37" s="1">
-        <v>49.816666666666698</v>
-      </c>
-      <c r="D37" s="1">
-        <v>5.0233696300000004</v>
-      </c>
+        <v>50.6</v>
+      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="2">
-        <v>44782</v>
+        <v>44779</v>
       </c>
       <c r="F37">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="G37">
-        <v>815</v>
+        <v>825</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1247,19 +1175,19 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>33.625</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="D38" s="1">
-        <v>6.7860987599999998</v>
+        <v>6.05685187</v>
       </c>
       <c r="E38" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F38">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G38">
-        <v>420</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1270,19 +1198,19 @@
         <v>2</v>
       </c>
       <c r="C39" s="1">
-        <v>44.141666666666701</v>
+        <v>47.966666666666697</v>
       </c>
       <c r="D39" s="1">
-        <v>3.6190049700000002</v>
+        <v>5.19446092</v>
       </c>
       <c r="E39" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F39">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G39">
-        <v>505</v>
+        <v>530</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1293,16 +1221,16 @@
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>53.3</v>
+        <v>53.058333333333302</v>
       </c>
       <c r="D40" s="1">
-        <v>4.3270817399999997</v>
+        <v>4.6097640100000001</v>
       </c>
       <c r="E40" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F40">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G40">
         <v>520</v>
@@ -1316,19 +1244,19 @@
         <v>4</v>
       </c>
       <c r="C41" s="1">
-        <v>33.558333333333302</v>
+        <v>42.358333333333299</v>
       </c>
       <c r="D41" s="1">
-        <v>5.1508972399999999</v>
+        <v>4.5197462399999999</v>
       </c>
       <c r="E41" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F41">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G41">
-        <v>435</v>
+        <v>480</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1339,19 +1267,19 @@
         <v>5</v>
       </c>
       <c r="C42" s="1">
-        <v>46.783333333333303</v>
+        <v>51.225000000000001</v>
       </c>
       <c r="D42" s="1">
-        <v>5.5815985499999998</v>
+        <v>4.0150002799999998</v>
       </c>
       <c r="E42" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F42">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G42">
-        <v>495</v>
+        <v>515</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1362,19 +1290,19 @@
         <v>6</v>
       </c>
       <c r="C43" s="1">
-        <v>51.65</v>
+        <v>52.5</v>
       </c>
       <c r="D43" s="1">
-        <v>3.5176180000000001</v>
+        <v>5.5891127899999997</v>
       </c>
       <c r="E43" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F43">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G43">
-        <v>540</v>
+        <v>545</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1385,19 +1313,19 @@
         <v>1</v>
       </c>
       <c r="C44" s="1">
-        <v>32.7083333333333</v>
+        <v>42.5416666666667</v>
       </c>
       <c r="D44" s="1">
-        <v>8.3195780399999997</v>
+        <v>4.7046318200000004</v>
       </c>
       <c r="E44" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F44">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G44">
-        <v>450</v>
+        <v>520</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1408,19 +1336,19 @@
         <v>2</v>
       </c>
       <c r="C45" s="1">
-        <v>49.366666666666703</v>
+        <v>53.5416666666667</v>
       </c>
       <c r="D45" s="1">
-        <v>10.204752300000001</v>
+        <v>6.8675069400000002</v>
       </c>
       <c r="E45" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F45">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G45">
-        <v>540</v>
+        <v>570</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1431,16 +1359,16 @@
         <v>3</v>
       </c>
       <c r="C46" s="1">
-        <v>59.391666666666701</v>
+        <v>59.183333333333302</v>
       </c>
       <c r="D46" s="1">
-        <v>3.2351642699999998</v>
+        <v>2.8837580699999998</v>
       </c>
       <c r="E46" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F46">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G46">
         <v>560</v>
@@ -1454,19 +1382,19 @@
         <v>4</v>
       </c>
       <c r="C47" s="1">
-        <v>36.35</v>
+        <v>43.241666666666703</v>
       </c>
       <c r="D47" s="1">
-        <v>7.6173844199999996</v>
+        <v>6.2950858700000003</v>
       </c>
       <c r="E47" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F47">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G47">
-        <v>440</v>
+        <v>490</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1477,19 +1405,19 @@
         <v>5</v>
       </c>
       <c r="C48" s="1">
-        <v>48.591666666666697</v>
+        <v>52.691666666666698</v>
       </c>
       <c r="D48" s="1">
-        <v>6.27222714</v>
+        <v>8.6660737000000001</v>
       </c>
       <c r="E48" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F48">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G48">
-        <v>540</v>
+        <v>570</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1500,19 +1428,19 @@
         <v>6</v>
       </c>
       <c r="C49" s="1">
-        <v>59.108333333333299</v>
+        <v>60.783333333333402</v>
       </c>
       <c r="D49" s="1">
-        <v>4.5595969399999996</v>
+        <v>2.1263854700000002</v>
       </c>
       <c r="E49" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F49">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G49">
-        <v>590</v>
+        <v>600</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1523,19 +1451,19 @@
         <v>1</v>
       </c>
       <c r="C50" s="1">
-        <v>23.816666666666698</v>
+        <v>32.766666666666701</v>
       </c>
       <c r="D50" s="1">
-        <v>7.52907496</v>
+        <v>7.4738736899999996</v>
       </c>
       <c r="E50" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F50">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G50">
-        <v>595</v>
+        <v>645</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1546,19 +1474,19 @@
         <v>2</v>
       </c>
       <c r="C51" s="1">
-        <v>37.591666666666697</v>
+        <v>43.008333333333297</v>
       </c>
       <c r="D51" s="1">
-        <v>5.4809518600000002</v>
+        <v>5.0579295699999998</v>
       </c>
       <c r="E51" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F51">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G51">
-        <v>685</v>
+        <v>710</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1569,19 +1497,19 @@
         <v>3</v>
       </c>
       <c r="C52" s="1">
-        <v>49.875</v>
+        <v>50.783333333333303</v>
       </c>
       <c r="D52" s="1">
-        <v>3.2133598999999999</v>
+        <v>3.1080052999999999</v>
       </c>
       <c r="E52" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F52">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G52">
-        <v>725</v>
+        <v>730</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1592,19 +1520,19 @@
         <v>4</v>
       </c>
       <c r="C53" s="1">
-        <v>16.691666666666698</v>
+        <v>23.316666666666698</v>
       </c>
       <c r="D53" s="1">
-        <v>6.4392910900000002</v>
+        <v>6.4566855199999997</v>
       </c>
       <c r="E53" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F53">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G53">
-        <v>585</v>
+        <v>625</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1615,19 +1543,19 @@
         <v>5</v>
       </c>
       <c r="C54" s="1">
-        <v>33.933333333333302</v>
+        <v>39.3333333333333</v>
       </c>
       <c r="D54" s="1">
-        <v>7.24234183</v>
+        <v>7.7572644400000001</v>
       </c>
       <c r="E54" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F54">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G54">
-        <v>700</v>
+        <v>720</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1638,19 +1566,19 @@
         <v>6</v>
       </c>
       <c r="C55" s="1">
-        <v>46.266666666666701</v>
+        <v>49.816666666666698</v>
       </c>
       <c r="D55" s="1">
-        <v>5.0517923600000003</v>
+        <v>5.0233696300000004</v>
       </c>
       <c r="E55" s="2">
-        <v>44784</v>
+        <v>44782</v>
       </c>
       <c r="F55">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G55">
-        <v>805</v>
+        <v>815</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1661,19 +1589,19 @@
         <v>1</v>
       </c>
       <c r="C56" s="1">
-        <v>30.524999999999999</v>
+        <v>33.625</v>
       </c>
       <c r="D56" s="1">
-        <v>8.0398015600000008</v>
+        <v>6.7860987599999998</v>
       </c>
       <c r="E56" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F56">
         <v>40</v>
       </c>
       <c r="G56">
-        <v>395</v>
+        <v>420</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1684,19 +1612,19 @@
         <v>2</v>
       </c>
       <c r="C57" s="1">
-        <v>39.858333333333299</v>
+        <v>44.141666666666701</v>
       </c>
       <c r="D57" s="1">
-        <v>6.9110528499999999</v>
+        <v>3.6190049700000002</v>
       </c>
       <c r="E57" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F57">
         <v>60</v>
       </c>
       <c r="G57">
-        <v>590</v>
+        <v>505</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1707,13 +1635,13 @@
         <v>3</v>
       </c>
       <c r="C58" s="1">
-        <v>48.95</v>
+        <v>53.3</v>
       </c>
       <c r="D58" s="1">
-        <v>6.43972049</v>
+        <v>4.3270817399999997</v>
       </c>
       <c r="E58" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F58">
         <v>80</v>
@@ -1730,19 +1658,19 @@
         <v>4</v>
       </c>
       <c r="C59" s="1">
-        <v>27.383333333333301</v>
+        <v>33.558333333333302</v>
       </c>
       <c r="D59" s="1">
-        <v>5.5838783100000002</v>
+        <v>5.1508972399999999</v>
       </c>
       <c r="E59" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F59">
         <v>40</v>
       </c>
       <c r="G59">
-        <v>400</v>
+        <v>435</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1753,19 +1681,19 @@
         <v>5</v>
       </c>
       <c r="C60" s="1">
-        <v>42.274999999999999</v>
+        <v>46.783333333333303</v>
       </c>
       <c r="D60" s="1">
-        <v>7.2376697700000001</v>
+        <v>5.5815985499999998</v>
       </c>
       <c r="E60" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F60">
         <v>60</v>
       </c>
       <c r="G60">
-        <v>480</v>
+        <v>495</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -1776,19 +1704,19 @@
         <v>6</v>
       </c>
       <c r="C61" s="1">
-        <v>48.883333333333297</v>
+        <v>51.65</v>
       </c>
       <c r="D61" s="1">
-        <v>4.8771887100000004</v>
+        <v>3.5176180000000001</v>
       </c>
       <c r="E61" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F61">
         <v>80</v>
       </c>
       <c r="G61">
-        <v>535</v>
+        <v>540</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1799,19 +1727,19 @@
         <v>1</v>
       </c>
       <c r="C62" s="1">
-        <v>27.633333333333301</v>
+        <v>32.7083333333333</v>
       </c>
       <c r="D62" s="1">
-        <v>8.6925603900000006</v>
+        <v>8.3195780399999997</v>
       </c>
       <c r="E62" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F62">
         <v>40</v>
       </c>
       <c r="G62">
-        <v>415</v>
+        <v>450</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -1822,19 +1750,19 @@
         <v>2</v>
       </c>
       <c r="C63" s="1">
-        <v>42.7</v>
+        <v>49.366666666666703</v>
       </c>
       <c r="D63" s="1">
-        <v>7.64852927</v>
+        <v>10.204752300000001</v>
       </c>
       <c r="E63" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F63">
         <v>60</v>
       </c>
       <c r="G63">
-        <v>515</v>
+        <v>540</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -1845,19 +1773,19 @@
         <v>3</v>
       </c>
       <c r="C64" s="1">
-        <v>59.466666666666697</v>
+        <v>59.391666666666701</v>
       </c>
       <c r="D64" s="1">
-        <v>3.30518417</v>
+        <v>3.2351642699999998</v>
       </c>
       <c r="E64" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F64">
         <v>80</v>
       </c>
       <c r="G64">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -1868,19 +1796,19 @@
         <v>4</v>
       </c>
       <c r="C65" s="1">
-        <v>29.1666666666667</v>
+        <v>36.35</v>
       </c>
       <c r="D65" s="1">
-        <v>8.2623277999999996</v>
+        <v>7.6173844199999996</v>
       </c>
       <c r="E65" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F65">
         <v>40</v>
       </c>
       <c r="G65">
-        <v>402</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -1891,19 +1819,19 @@
         <v>5</v>
       </c>
       <c r="C66" s="1">
-        <v>44.1666666666667</v>
+        <v>48.591666666666697</v>
       </c>
       <c r="D66" s="1">
-        <v>6.5887415499999999</v>
+        <v>6.27222714</v>
       </c>
       <c r="E66" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F66">
         <v>60</v>
       </c>
       <c r="G66">
-        <v>515</v>
+        <v>540</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -1914,13 +1842,13 @@
         <v>6</v>
       </c>
       <c r="C67" s="1">
-        <v>60.741666666666703</v>
+        <v>59.108333333333299</v>
       </c>
       <c r="D67" s="1">
-        <v>2.4126403199999999</v>
+        <v>4.5595969399999996</v>
       </c>
       <c r="E67" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F67">
         <v>80</v>
@@ -1937,19 +1865,19 @@
         <v>1</v>
       </c>
       <c r="C68" s="1">
-        <v>18.308333333333302</v>
+        <v>23.816666666666698</v>
       </c>
       <c r="D68" s="1">
-        <v>7.15827028</v>
+        <v>7.52907496</v>
       </c>
       <c r="E68" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F68">
         <v>40</v>
       </c>
       <c r="G68">
-        <v>570</v>
+        <v>595</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -1960,19 +1888,19 @@
         <v>2</v>
       </c>
       <c r="C69" s="1">
-        <v>33.125</v>
+        <v>37.591666666666697</v>
       </c>
       <c r="D69" s="1">
-        <v>7.6243777699999997</v>
+        <v>5.4809518600000002</v>
       </c>
       <c r="E69" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F69">
         <v>60</v>
       </c>
       <c r="G69">
-        <v>665</v>
+        <v>685</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -1983,13 +1911,13 @@
         <v>3</v>
       </c>
       <c r="C70" s="1">
-        <v>48.841666666666697</v>
+        <v>49.875</v>
       </c>
       <c r="D70" s="1">
-        <v>3.23038369</v>
+        <v>3.2133598999999999</v>
       </c>
       <c r="E70" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F70">
         <v>80</v>
@@ -2006,19 +1934,19 @@
         <v>4</v>
       </c>
       <c r="C71" s="1">
-        <v>13.8166666666667</v>
+        <v>16.691666666666698</v>
       </c>
       <c r="D71" s="1">
-        <v>5.99800472</v>
+        <v>6.4392910900000002</v>
       </c>
       <c r="E71" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F71">
         <v>40</v>
       </c>
       <c r="G71">
-        <v>565</v>
+        <v>585</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2029,19 +1957,19 @@
         <v>5</v>
       </c>
       <c r="C72" s="1">
-        <v>32.0833333333333</v>
+        <v>33.933333333333302</v>
       </c>
       <c r="D72" s="1">
-        <v>8.4126347999999993</v>
+        <v>7.24234183</v>
       </c>
       <c r="E72" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F72">
         <v>60</v>
       </c>
       <c r="G72">
-        <v>680</v>
+        <v>700</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2052,19 +1980,19 @@
         <v>6</v>
       </c>
       <c r="C73" s="1">
-        <v>43.966666666666697</v>
+        <v>46.266666666666701</v>
       </c>
       <c r="D73" s="1">
-        <v>7.2891367899999997</v>
+        <v>5.0517923600000003</v>
       </c>
       <c r="E73" s="2">
-        <v>44786</v>
+        <v>44784</v>
       </c>
       <c r="F73">
         <v>80</v>
       </c>
       <c r="G73">
-        <v>792</v>
+        <v>805</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2075,19 +2003,19 @@
         <v>1</v>
       </c>
       <c r="C74" s="1">
-        <v>22.875</v>
+        <v>30.524999999999999</v>
       </c>
       <c r="D74" s="1">
-        <v>7.0606624699999996</v>
+        <v>8.0398015600000008</v>
       </c>
       <c r="E74" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F74">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G74">
-        <v>340</v>
+        <v>395</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2098,19 +2026,19 @@
         <v>2</v>
       </c>
       <c r="C75" s="1">
-        <v>33.4</v>
+        <v>39.858333333333299</v>
       </c>
       <c r="D75" s="1">
-        <v>6.6130724499999998</v>
+        <v>6.9110528499999999</v>
       </c>
       <c r="E75" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F75">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G75">
-        <v>430</v>
+        <v>590</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2121,19 +2049,19 @@
         <v>3</v>
       </c>
       <c r="C76" s="1">
-        <v>45.825000000000003</v>
+        <v>48.95</v>
       </c>
       <c r="D76" s="1">
-        <v>9.1952680499999992</v>
+        <v>6.43972049</v>
       </c>
       <c r="E76" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F76">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G76">
-        <v>505</v>
+        <v>520</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2144,19 +2072,19 @@
         <v>4</v>
       </c>
       <c r="C77" s="1">
-        <v>19.216666666666701</v>
+        <v>27.383333333333301</v>
       </c>
       <c r="D77" s="1">
-        <v>5.5579318200000003</v>
+        <v>5.5838783100000002</v>
       </c>
       <c r="E77" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F77">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G77">
-        <v>332</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2167,19 +2095,19 @@
         <v>5</v>
       </c>
       <c r="C78" s="1">
-        <v>34.325000000000003</v>
+        <v>42.274999999999999</v>
       </c>
       <c r="D78" s="1">
-        <v>6.7669148300000002</v>
+        <v>7.2376697700000001</v>
       </c>
       <c r="E78" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F78">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G78">
-        <v>425</v>
+        <v>480</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2190,19 +2118,19 @@
         <v>6</v>
       </c>
       <c r="C79" s="1">
-        <v>43.408333333333303</v>
+        <v>48.883333333333297</v>
       </c>
       <c r="D79" s="1">
-        <v>9.05784023</v>
+        <v>4.8771887100000004</v>
       </c>
       <c r="E79" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F79">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G79">
-        <v>500</v>
+        <v>535</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -2213,19 +2141,19 @@
         <v>1</v>
       </c>
       <c r="C80" s="1">
-        <v>16.466666666666701</v>
+        <v>27.633333333333301</v>
       </c>
       <c r="D80" s="1">
-        <v>6.0572020699999998</v>
+        <v>8.6925603900000006</v>
       </c>
       <c r="E80" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F80">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G80">
-        <v>350</v>
+        <v>415</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -2236,19 +2164,19 @@
         <v>2</v>
       </c>
       <c r="C81" s="1">
-        <v>32.616666666666703</v>
+        <v>42.7</v>
       </c>
       <c r="D81" s="1">
-        <v>8.8217534200000003</v>
+        <v>7.64852927</v>
       </c>
       <c r="E81" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F81">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G81">
-        <v>450</v>
+        <v>515</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2259,19 +2187,19 @@
         <v>3</v>
       </c>
       <c r="C82" s="1">
-        <v>51.25</v>
+        <v>59.466666666666697</v>
       </c>
       <c r="D82" s="1">
-        <v>4.8451475300000002</v>
+        <v>3.30518417</v>
       </c>
       <c r="E82" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F82">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G82">
-        <v>530</v>
+        <v>555</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -2282,19 +2210,19 @@
         <v>4</v>
       </c>
       <c r="C83" s="1">
-        <v>16.008333333333301</v>
+        <v>29.1666666666667</v>
       </c>
       <c r="D83" s="1">
-        <v>6.1424688999999999</v>
+        <v>8.2623277999999996</v>
       </c>
       <c r="E83" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F83">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G83">
-        <v>330</v>
+        <v>402</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -2305,19 +2233,19 @@
         <v>5</v>
       </c>
       <c r="C84" s="1">
-        <v>32.049999999999997</v>
+        <v>44.1666666666667</v>
       </c>
       <c r="D84" s="1">
-        <v>7.7857095200000002</v>
+        <v>6.5887415499999999</v>
       </c>
       <c r="E84" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F84">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G84">
-        <v>442</v>
+        <v>515</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -2328,19 +2256,19 @@
         <v>6</v>
       </c>
       <c r="C85" s="1">
-        <v>52</v>
+        <v>60.741666666666703</v>
       </c>
       <c r="D85" s="1">
-        <v>3.3709993100000002</v>
+        <v>2.4126403199999999</v>
       </c>
       <c r="E85" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F85">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G85">
-        <v>550</v>
+        <v>590</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -2351,19 +2279,19 @@
         <v>1</v>
       </c>
       <c r="C86" s="1">
-        <v>11.158333333333299</v>
+        <v>18.308333333333302</v>
       </c>
       <c r="D86" s="1">
-        <v>4.6052259500000003</v>
+        <v>7.15827028</v>
       </c>
       <c r="E86" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F86">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G86">
-        <v>515</v>
+        <v>570</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -2374,19 +2302,19 @@
         <v>2</v>
       </c>
       <c r="C87" s="1">
-        <v>22.925000000000001</v>
+        <v>33.125</v>
       </c>
       <c r="D87" s="1">
-        <v>6.8871586699999998</v>
+        <v>7.6243777699999997</v>
       </c>
       <c r="E87" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F87">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G87">
-        <v>602</v>
+        <v>665</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -2397,19 +2325,19 @@
         <v>3</v>
       </c>
       <c r="C88" s="1">
-        <v>42.424999999999997</v>
+        <v>48.841666666666697</v>
       </c>
       <c r="D88" s="1">
-        <v>4.8727675499999998</v>
+        <v>3.23038369</v>
       </c>
       <c r="E88" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F88">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G88">
-        <v>700</v>
+        <v>725</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -2420,19 +2348,19 @@
         <v>4</v>
       </c>
       <c r="C89" s="1">
-        <v>8.625</v>
+        <v>13.8166666666667</v>
       </c>
       <c r="D89" s="1">
-        <v>2.4521326499999998</v>
+        <v>5.99800472</v>
       </c>
       <c r="E89" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F89">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G89">
-        <v>520</v>
+        <v>565</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -2443,19 +2371,19 @@
         <v>5</v>
       </c>
       <c r="C90" s="1">
-        <v>23.866666666666699</v>
+        <v>32.0833333333333</v>
       </c>
       <c r="D90" s="1">
-        <v>9.4161692000000006</v>
+        <v>8.4126347999999993</v>
       </c>
       <c r="E90" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F90">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G90">
-        <v>625</v>
+        <v>680</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -2466,19 +2394,19 @@
         <v>6</v>
       </c>
       <c r="C91" s="1">
-        <v>34.299999999999997</v>
+        <v>43.966666666666697</v>
       </c>
       <c r="D91" s="1">
-        <v>6.2087914199999998</v>
+        <v>7.2891367899999997</v>
       </c>
       <c r="E91" s="2">
-        <v>44789</v>
+        <v>44786</v>
       </c>
       <c r="F91">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G91">
-        <v>735</v>
+        <v>792</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -2489,19 +2417,19 @@
         <v>1</v>
       </c>
       <c r="C92" s="1">
-        <v>13.4583333333333</v>
+        <v>22.875</v>
       </c>
       <c r="D92" s="1">
-        <v>5.8033624000000001</v>
+        <v>7.0606624699999996</v>
       </c>
       <c r="E92" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F92">
         <v>30</v>
       </c>
       <c r="G92">
-        <v>282</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -2512,19 +2440,19 @@
         <v>2</v>
       </c>
       <c r="C93" s="1">
-        <v>22.324999999999999</v>
+        <v>33.4</v>
       </c>
       <c r="D93" s="1">
-        <v>6.1614822599999997</v>
+        <v>6.6130724499999998</v>
       </c>
       <c r="E93" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F93">
         <v>45</v>
       </c>
       <c r="G93">
-        <v>365</v>
+        <v>430</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -2535,19 +2463,19 @@
         <v>3</v>
       </c>
       <c r="C94" s="1">
-        <v>36.608333333333299</v>
+        <v>45.825000000000003</v>
       </c>
       <c r="D94" s="1">
-        <v>8.6130406799999992</v>
+        <v>9.1952680499999992</v>
       </c>
       <c r="E94" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F94">
         <v>60</v>
       </c>
       <c r="G94">
-        <v>442</v>
+        <v>505</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -2558,19 +2486,19 @@
         <v>4</v>
       </c>
       <c r="C95" s="1">
-        <v>11.741666666666699</v>
+        <v>19.216666666666701</v>
       </c>
       <c r="D95" s="1">
-        <v>3.84008957</v>
+        <v>5.5579318200000003</v>
       </c>
       <c r="E95" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F95">
         <v>30</v>
       </c>
       <c r="G95">
-        <v>275</v>
+        <v>332</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -2581,19 +2509,19 @@
         <v>5</v>
       </c>
       <c r="C96" s="1">
-        <v>24.875</v>
+        <v>34.325000000000003</v>
       </c>
       <c r="D96" s="1">
-        <v>5.5447149299999996</v>
+        <v>6.7669148300000002</v>
       </c>
       <c r="E96" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F96">
         <v>45</v>
       </c>
       <c r="G96">
-        <v>360</v>
+        <v>425</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -2604,19 +2532,19 @@
         <v>6</v>
       </c>
       <c r="C97" s="1">
-        <v>33.2083333333333</v>
+        <v>43.408333333333303</v>
       </c>
       <c r="D97" s="1">
-        <v>9.7817509400000002</v>
+        <v>9.05784023</v>
       </c>
       <c r="E97" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F97">
         <v>60</v>
       </c>
       <c r="G97">
-        <v>430</v>
+        <v>500</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -2627,19 +2555,19 @@
         <v>1</v>
       </c>
       <c r="C98" s="1">
-        <v>11.366666666666699</v>
+        <v>16.466666666666701</v>
       </c>
       <c r="D98" s="1">
-        <v>4.7105941199999997</v>
+        <v>6.0572020699999998</v>
       </c>
       <c r="E98" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F98">
         <v>30</v>
       </c>
       <c r="G98">
-        <v>300</v>
+        <v>350</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -2650,19 +2578,19 @@
         <v>2</v>
       </c>
       <c r="C99" s="1">
-        <v>20.933333333333302</v>
+        <v>32.616666666666703</v>
       </c>
       <c r="D99" s="1">
-        <v>8.86385237</v>
+        <v>8.8217534200000003</v>
       </c>
       <c r="E99" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F99">
         <v>45</v>
       </c>
       <c r="G99">
-        <v>375</v>
+        <v>450</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -2673,19 +2601,19 @@
         <v>3</v>
       </c>
       <c r="C100" s="1">
-        <v>41.358333333333299</v>
+        <v>51.25</v>
       </c>
       <c r="D100" s="1">
-        <v>5.2184042000000002</v>
+        <v>4.8451475300000002</v>
       </c>
       <c r="E100" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F100">
         <v>60</v>
       </c>
       <c r="G100">
-        <v>470</v>
+        <v>530</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -2696,19 +2624,19 @@
         <v>4</v>
       </c>
       <c r="C101" s="1">
-        <v>9.4</v>
+        <v>16.008333333333301</v>
       </c>
       <c r="D101" s="1">
-        <v>3.5386181200000002</v>
+        <v>6.1424688999999999</v>
       </c>
       <c r="E101" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F101">
         <v>30</v>
       </c>
       <c r="G101">
-        <v>275</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -2719,19 +2647,19 @@
         <v>5</v>
       </c>
       <c r="C102" s="1">
-        <v>19.074999999999999</v>
+        <v>32.049999999999997</v>
       </c>
       <c r="D102" s="1">
-        <v>6.5026043700000002</v>
+        <v>7.7857095200000002</v>
       </c>
       <c r="E102" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F102">
         <v>45</v>
       </c>
       <c r="G102">
-        <v>362</v>
+        <v>442</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -2742,19 +2670,19 @@
         <v>6</v>
       </c>
       <c r="C103" s="1">
-        <v>39.966666666666697</v>
+        <v>52</v>
       </c>
       <c r="D103" s="1">
-        <v>4.9545816</v>
+        <v>3.3709993100000002</v>
       </c>
       <c r="E103" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F103">
         <v>60</v>
       </c>
       <c r="G103">
-        <v>480</v>
+        <v>550</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -2765,19 +2693,19 @@
         <v>1</v>
       </c>
       <c r="C104" s="1">
-        <v>7.4083333333333297</v>
+        <v>11.158333333333299</v>
       </c>
       <c r="D104" s="1">
-        <v>2.47439922</v>
+        <v>4.6052259500000003</v>
       </c>
       <c r="E104" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F104">
         <v>30</v>
       </c>
       <c r="G104">
-        <v>478</v>
+        <v>515</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -2788,19 +2716,19 @@
         <v>2</v>
       </c>
       <c r="C105" s="1">
-        <v>12.383333333333301</v>
+        <v>22.925000000000001</v>
       </c>
       <c r="D105" s="1">
-        <v>4.0260138899999998</v>
+        <v>6.8871586699999998</v>
       </c>
       <c r="E105" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F105">
         <v>45</v>
       </c>
       <c r="G105">
-        <v>530</v>
+        <v>602</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -2811,19 +2739,19 @@
         <v>3</v>
       </c>
       <c r="C106" s="1">
-        <v>29.6</v>
+        <v>42.424999999999997</v>
       </c>
       <c r="D106" s="1">
-        <v>4.42122978</v>
+        <v>4.8727675499999998</v>
       </c>
       <c r="E106" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F106">
         <v>60</v>
       </c>
       <c r="G106">
-        <v>631</v>
+        <v>700</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -2834,19 +2762,19 @@
         <v>4</v>
       </c>
       <c r="C107" s="1">
-        <v>5.9749999999999996</v>
+        <v>8.625</v>
       </c>
       <c r="D107" s="1">
-        <v>2.4391224199999999</v>
+        <v>2.4521326499999998</v>
       </c>
       <c r="E107" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F107">
         <v>30</v>
       </c>
       <c r="G107">
-        <v>492</v>
+        <v>520</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -2857,19 +2785,19 @@
         <v>5</v>
       </c>
       <c r="C108" s="1">
-        <v>14.591666666666701</v>
+        <v>23.866666666666699</v>
       </c>
       <c r="D108" s="1">
-        <v>6.1691989100000004</v>
+        <v>9.4161692000000006</v>
       </c>
       <c r="E108" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F108">
         <v>45</v>
       </c>
       <c r="G108">
-        <v>565</v>
+        <v>625</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -2880,19 +2808,19 @@
         <v>6</v>
       </c>
       <c r="C109" s="1">
-        <v>22.741666666666699</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D109" s="1">
-        <v>5.7722625699999996</v>
+        <v>6.2087914199999998</v>
       </c>
       <c r="E109" s="2">
-        <v>44791</v>
+        <v>44789</v>
       </c>
       <c r="F109">
         <v>60</v>
       </c>
       <c r="G109">
-        <v>652</v>
+        <v>735</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -2903,19 +2831,19 @@
         <v>1</v>
       </c>
       <c r="C110" s="1">
-        <v>11.283333333333299</v>
+        <v>13.4583333333333</v>
       </c>
       <c r="D110" s="1">
-        <v>4.0426888700000001</v>
+        <v>5.8033624000000001</v>
       </c>
       <c r="E110" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F110">
         <v>30</v>
       </c>
       <c r="G110">
-        <v>255</v>
+        <v>282</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -2926,19 +2854,19 @@
         <v>2</v>
       </c>
       <c r="C111" s="1">
-        <v>18.266666666666701</v>
+        <v>22.324999999999999</v>
       </c>
       <c r="D111" s="1">
-        <v>6.4715227000000004</v>
+        <v>6.1614822599999997</v>
       </c>
       <c r="E111" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F111">
         <v>45</v>
       </c>
       <c r="G111">
-        <v>335</v>
+        <v>365</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -2949,19 +2877,19 @@
         <v>3</v>
       </c>
       <c r="C112" s="1">
-        <v>28.774999999999999</v>
+        <v>36.608333333333299</v>
       </c>
       <c r="D112" s="1">
-        <v>10.5458415</v>
+        <v>8.6130406799999992</v>
       </c>
       <c r="E112" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F112">
         <v>60</v>
       </c>
       <c r="G112">
-        <v>420</v>
+        <v>442</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
@@ -2972,19 +2900,19 @@
         <v>4</v>
       </c>
       <c r="C113" s="1">
-        <v>9.0749999999999993</v>
+        <v>11.741666666666699</v>
       </c>
       <c r="D113" s="1">
-        <v>6.5744858099999997</v>
+        <v>3.84008957</v>
       </c>
       <c r="E113" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F113">
         <v>30</v>
       </c>
       <c r="G113">
-        <v>250</v>
+        <v>275</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -2995,19 +2923,19 @@
         <v>5</v>
       </c>
       <c r="C114" s="1">
-        <v>21.108333333333299</v>
+        <v>24.875</v>
       </c>
       <c r="D114" s="1">
-        <v>4.77311759</v>
+        <v>5.5447149299999996</v>
       </c>
       <c r="E114" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F114">
         <v>45</v>
       </c>
       <c r="G114">
-        <v>322</v>
+        <v>360</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -3018,19 +2946,19 @@
         <v>6</v>
       </c>
       <c r="C115" s="1">
-        <v>28.0833333333333</v>
+        <v>33.2083333333333</v>
       </c>
       <c r="D115" s="1">
-        <v>7.6162306800000001</v>
+        <v>9.7817509400000002</v>
       </c>
       <c r="E115" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F115">
         <v>60</v>
       </c>
       <c r="G115">
-        <v>382</v>
+        <v>430</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -3041,19 +2969,19 @@
         <v>1</v>
       </c>
       <c r="C116" s="1">
-        <v>9.1083333333333307</v>
+        <v>11.366666666666699</v>
       </c>
       <c r="D116" s="1">
-        <v>4.0078237899999998</v>
+        <v>4.7105941199999997</v>
       </c>
       <c r="E116" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F116">
         <v>30</v>
       </c>
       <c r="G116">
-        <v>270</v>
+        <v>300</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -3064,19 +2992,19 @@
         <v>2</v>
       </c>
       <c r="C117" s="1">
-        <v>16.324999999999999</v>
+        <v>20.933333333333302</v>
       </c>
       <c r="D117" s="1">
-        <v>7.5141230700000001</v>
+        <v>8.86385237</v>
       </c>
       <c r="E117" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F117">
         <v>45</v>
       </c>
       <c r="G117">
-        <v>337</v>
+        <v>375</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -3087,19 +3015,19 @@
         <v>3</v>
       </c>
       <c r="C118" s="1">
-        <v>34.391666666666701</v>
+        <v>41.358333333333299</v>
       </c>
       <c r="D118" s="1">
-        <v>7.6958617399999998</v>
+        <v>5.2184042000000002</v>
       </c>
       <c r="E118" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F118">
         <v>60</v>
       </c>
       <c r="G118">
-        <v>425</v>
+        <v>470</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -3110,19 +3038,19 @@
         <v>4</v>
       </c>
       <c r="C119" s="1">
-        <v>7.9166666666666696</v>
+        <v>9.4</v>
       </c>
       <c r="D119" s="1">
-        <v>4.0099497499999996</v>
+        <v>3.5386181200000002</v>
       </c>
       <c r="E119" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F119">
         <v>30</v>
       </c>
       <c r="G119">
-        <v>245</v>
+        <v>275</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -3133,19 +3061,19 @@
         <v>5</v>
       </c>
       <c r="C120" s="1">
-        <v>15.233333333333301</v>
+        <v>19.074999999999999</v>
       </c>
       <c r="D120" s="1">
-        <v>5.2865753399999997</v>
+        <v>6.5026043700000002</v>
       </c>
       <c r="E120" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F120">
         <v>45</v>
       </c>
       <c r="G120">
-        <v>322</v>
+        <v>362</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -3156,19 +3084,19 @@
         <v>6</v>
       </c>
       <c r="C121" s="1">
-        <v>32.7083333333333</v>
+        <v>39.966666666666697</v>
       </c>
       <c r="D121" s="1">
-        <v>10.2219424</v>
+        <v>4.9545816</v>
       </c>
       <c r="E121" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F121">
         <v>60</v>
       </c>
       <c r="G121">
-        <v>431</v>
+        <v>480</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -3179,19 +3107,19 @@
         <v>1</v>
       </c>
       <c r="C122" s="1">
-        <v>5.30833333333333</v>
+        <v>7.4083333333333297</v>
       </c>
       <c r="D122" s="1">
-        <v>1.7095764099999999</v>
+        <v>2.47439922</v>
       </c>
       <c r="E122" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F122">
         <v>30</v>
       </c>
       <c r="G122">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -3202,19 +3130,19 @@
         <v>2</v>
       </c>
       <c r="C123" s="1">
-        <v>9.55833333333333</v>
+        <v>12.383333333333301</v>
       </c>
       <c r="D123" s="1">
-        <v>2.8477928700000001</v>
+        <v>4.0260138899999998</v>
       </c>
       <c r="E123" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F123">
         <v>45</v>
       </c>
       <c r="G123">
-        <v>500</v>
+        <v>530</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -3225,19 +3153,19 @@
         <v>3</v>
       </c>
       <c r="C124" s="1">
-        <v>24.9166666666667</v>
+        <v>29.6</v>
       </c>
       <c r="D124" s="1">
-        <v>6.9137324900000001</v>
+        <v>4.42122978</v>
       </c>
       <c r="E124" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F124">
         <v>60</v>
       </c>
       <c r="G124">
-        <v>591</v>
+        <v>631</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -3248,19 +3176,19 @@
         <v>4</v>
       </c>
       <c r="C125" s="1">
-        <v>5.0333333333333297</v>
+        <v>5.9749999999999996</v>
       </c>
       <c r="D125" s="1">
-        <v>2.2202920900000001</v>
+        <v>2.4391224199999999</v>
       </c>
       <c r="E125" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F125">
         <v>30</v>
       </c>
       <c r="G125">
-        <v>455</v>
+        <v>492</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -3271,19 +3199,19 @@
         <v>5</v>
       </c>
       <c r="C126" s="1">
-        <v>11.1916666666667</v>
+        <v>14.591666666666701</v>
       </c>
       <c r="D126" s="1">
-        <v>3.4431640699999999</v>
+        <v>6.1691989100000004</v>
       </c>
       <c r="E126" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F126">
         <v>45</v>
       </c>
       <c r="G126">
-        <v>535</v>
+        <v>565</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
@@ -3294,19 +3222,19 @@
         <v>6</v>
       </c>
       <c r="C127" s="1">
-        <v>16.758333333333301</v>
+        <v>22.741666666666699</v>
       </c>
       <c r="D127" s="1">
-        <v>5.8050852800000001</v>
+        <v>5.7722625699999996</v>
       </c>
       <c r="E127" s="2">
-        <v>44793</v>
+        <v>44791</v>
       </c>
       <c r="F127">
         <v>60</v>
       </c>
       <c r="G127">
-        <v>605</v>
+        <v>652</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
@@ -3317,19 +3245,19 @@
         <v>1</v>
       </c>
       <c r="C128" s="1">
-        <v>9.0666666666666593</v>
+        <v>11.283333333333299</v>
       </c>
       <c r="D128" s="1">
-        <v>4.3267315699999997</v>
+        <v>4.0426888700000001</v>
       </c>
       <c r="E128" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F128">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G128">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
@@ -3340,19 +3268,19 @@
         <v>2</v>
       </c>
       <c r="C129" s="1">
-        <v>17.5</v>
+        <v>18.266666666666701</v>
       </c>
       <c r="D129" s="1">
-        <v>6.6420150299999996</v>
+        <v>6.4715227000000004</v>
       </c>
       <c r="E129" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F129">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G129">
-        <v>325</v>
+        <v>335</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
@@ -3363,19 +3291,19 @@
         <v>3</v>
       </c>
       <c r="C130" s="1">
-        <v>33.15</v>
+        <v>28.774999999999999</v>
       </c>
       <c r="D130" s="1">
-        <v>9.6141467699999996</v>
+        <v>10.5458415</v>
       </c>
       <c r="E130" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F130">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G130">
-        <v>405</v>
+        <v>420</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
@@ -3386,19 +3314,19 @@
         <v>4</v>
       </c>
       <c r="C131" s="1">
-        <v>7.3916666666666702</v>
+        <v>9.0749999999999993</v>
       </c>
       <c r="D131" s="1">
-        <v>4.1491419299999999</v>
+        <v>6.5744858099999997</v>
       </c>
       <c r="E131" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F131">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G131">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
@@ -3409,19 +3337,19 @@
         <v>5</v>
       </c>
       <c r="C132" s="1">
-        <v>18.2916666666667</v>
+        <v>21.108333333333299</v>
       </c>
       <c r="D132" s="1">
-        <v>5.3595214100000002</v>
+        <v>4.77311759</v>
       </c>
       <c r="E132" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F132">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G132">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -3432,19 +3360,19 @@
         <v>6</v>
       </c>
       <c r="C133" s="1">
-        <v>25.983333333333299</v>
+        <v>28.0833333333333</v>
       </c>
       <c r="D133" s="1">
-        <v>8.5988195100000002</v>
+        <v>7.6162306800000001</v>
       </c>
       <c r="E133" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F133">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G133">
-        <v>375</v>
+        <v>382</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -3455,19 +3383,19 @@
         <v>1</v>
       </c>
       <c r="C134" s="1">
-        <v>9.0166666666666693</v>
+        <v>9.1083333333333307</v>
       </c>
       <c r="D134" s="1">
-        <v>3.0234938599999999</v>
+        <v>4.0078237899999998</v>
       </c>
       <c r="E134" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F134">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G134">
-        <v>260</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -3478,19 +3406,19 @@
         <v>2</v>
       </c>
       <c r="C135" s="1">
-        <v>14.6916666666667</v>
+        <v>16.324999999999999</v>
       </c>
       <c r="D135" s="1">
-        <v>5.5299939699999996</v>
+        <v>7.5141230700000001</v>
       </c>
       <c r="E135" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F135">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G135">
-        <v>325</v>
+        <v>337</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
@@ -3501,19 +3429,19 @@
         <v>3</v>
       </c>
       <c r="C136" s="1">
-        <v>33.725000000000001</v>
+        <v>34.391666666666701</v>
       </c>
       <c r="D136" s="1">
-        <v>10.120287899999999</v>
+        <v>7.6958617399999998</v>
       </c>
       <c r="E136" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F136">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G136">
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
@@ -3524,19 +3452,19 @@
         <v>4</v>
       </c>
       <c r="C137" s="1">
-        <v>8.4916666666666707</v>
+        <v>7.9166666666666696</v>
       </c>
       <c r="D137" s="1">
-        <v>4.81559179</v>
+        <v>4.0099497499999996</v>
       </c>
       <c r="E137" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F137">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G137">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
@@ -3547,19 +3475,19 @@
         <v>5</v>
       </c>
       <c r="C138" s="1">
-        <v>13.225</v>
+        <v>15.233333333333301</v>
       </c>
       <c r="D138" s="1">
-        <v>4.6331071499999998</v>
+        <v>5.2865753399999997</v>
       </c>
       <c r="E138" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F138">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G138">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
@@ -3570,19 +3498,19 @@
         <v>6</v>
       </c>
       <c r="C139" s="1">
-        <v>30.941666666666698</v>
+        <v>32.7083333333333</v>
       </c>
       <c r="D139" s="1">
-        <v>12.5605051</v>
+        <v>10.2219424</v>
       </c>
       <c r="E139" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F139">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G139">
-        <v>420</v>
+        <v>431</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
@@ -3593,19 +3521,19 @@
         <v>1</v>
       </c>
       <c r="C140" s="1">
-        <v>5.4666666666666703</v>
+        <v>5.30833333333333</v>
       </c>
       <c r="D140" s="1">
-        <v>2.6776289800000002</v>
+        <v>1.7095764099999999</v>
       </c>
       <c r="E140" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F140">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G140">
-        <v>472</v>
+        <v>480</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
@@ -3616,19 +3544,19 @@
         <v>2</v>
       </c>
       <c r="C141" s="1">
-        <v>8.9083333333333297</v>
+        <v>9.55833333333333</v>
       </c>
       <c r="D141" s="1">
-        <v>3.2814792499999998</v>
+        <v>2.8477928700000001</v>
       </c>
       <c r="E141" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F141">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G141">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
@@ -3639,19 +3567,19 @@
         <v>3</v>
       </c>
       <c r="C142" s="1">
-        <v>21.975000000000001</v>
+        <v>24.9166666666667</v>
       </c>
       <c r="D142" s="1">
-        <v>9.1335669599999996</v>
+        <v>6.9137324900000001</v>
       </c>
       <c r="E142" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F142">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G142">
-        <v>580</v>
+        <v>591</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
@@ -3662,16 +3590,16 @@
         <v>4</v>
       </c>
       <c r="C143" s="1">
-        <v>6.0916666666666703</v>
+        <v>5.0333333333333297</v>
       </c>
       <c r="D143" s="1">
-        <v>2.81633493</v>
+        <v>2.2202920900000001</v>
       </c>
       <c r="E143" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F143">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G143">
         <v>455</v>
@@ -3685,19 +3613,19 @@
         <v>5</v>
       </c>
       <c r="C144" s="1">
-        <v>9.2750000000000004</v>
+        <v>11.1916666666667</v>
       </c>
       <c r="D144" s="1">
-        <v>3.4892367000000002</v>
+        <v>3.4431640699999999</v>
       </c>
       <c r="E144" s="2">
-        <v>44796</v>
+        <v>44793</v>
       </c>
       <c r="F144">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G144">
-        <v>530</v>
+        <v>535</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
@@ -3708,18 +3636,432 @@
         <v>6</v>
       </c>
       <c r="C145" s="1">
+        <v>16.758333333333301</v>
+      </c>
+      <c r="D145" s="1">
+        <v>5.8050852800000001</v>
+      </c>
+      <c r="E145" s="2">
+        <v>44793</v>
+      </c>
+      <c r="F145">
+        <v>60</v>
+      </c>
+      <c r="G145">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146" s="1">
+        <v>9.0666666666666593</v>
+      </c>
+      <c r="D146" s="1">
+        <v>4.3267315699999997</v>
+      </c>
+      <c r="E146" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F146">
+        <v>50</v>
+      </c>
+      <c r="G146">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>2</v>
+      </c>
+      <c r="C147" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="D147" s="1">
+        <v>6.6420150299999996</v>
+      </c>
+      <c r="E147" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F147">
+        <v>50</v>
+      </c>
+      <c r="G147">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>3</v>
+      </c>
+      <c r="C148" s="1">
+        <v>33.15</v>
+      </c>
+      <c r="D148" s="1">
+        <v>9.6141467699999996</v>
+      </c>
+      <c r="E148" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F148">
+        <v>50</v>
+      </c>
+      <c r="G148">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>4</v>
+      </c>
+      <c r="C149" s="1">
+        <v>7.3916666666666702</v>
+      </c>
+      <c r="D149" s="1">
+        <v>4.1491419299999999</v>
+      </c>
+      <c r="E149" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F149">
+        <v>50</v>
+      </c>
+      <c r="G149">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
+        <v>5</v>
+      </c>
+      <c r="C150" s="1">
+        <v>18.2916666666667</v>
+      </c>
+      <c r="D150" s="1">
+        <v>5.3595214100000002</v>
+      </c>
+      <c r="E150" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F150">
+        <v>50</v>
+      </c>
+      <c r="G150">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>6</v>
+      </c>
+      <c r="C151" s="1">
+        <v>25.983333333333299</v>
+      </c>
+      <c r="D151" s="1">
+        <v>8.5988195100000002</v>
+      </c>
+      <c r="E151" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F151">
+        <v>50</v>
+      </c>
+      <c r="G151">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>2</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152" s="1">
+        <v>9.0166666666666693</v>
+      </c>
+      <c r="D152" s="1">
+        <v>3.0234938599999999</v>
+      </c>
+      <c r="E152" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F152">
+        <v>50</v>
+      </c>
+      <c r="G152">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>2</v>
+      </c>
+      <c r="B153">
+        <v>2</v>
+      </c>
+      <c r="C153" s="1">
+        <v>14.6916666666667</v>
+      </c>
+      <c r="D153" s="1">
+        <v>5.5299939699999996</v>
+      </c>
+      <c r="E153" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F153">
+        <v>50</v>
+      </c>
+      <c r="G153">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>2</v>
+      </c>
+      <c r="B154">
+        <v>3</v>
+      </c>
+      <c r="C154" s="1">
+        <v>33.725000000000001</v>
+      </c>
+      <c r="D154" s="1">
+        <v>10.120287899999999</v>
+      </c>
+      <c r="E154" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F154">
+        <v>50</v>
+      </c>
+      <c r="G154">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>2</v>
+      </c>
+      <c r="B155">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1">
+        <v>8.4916666666666707</v>
+      </c>
+      <c r="D155" s="1">
+        <v>4.81559179</v>
+      </c>
+      <c r="E155" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F155">
+        <v>50</v>
+      </c>
+      <c r="G155">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>2</v>
+      </c>
+      <c r="B156">
+        <v>5</v>
+      </c>
+      <c r="C156" s="1">
+        <v>13.225</v>
+      </c>
+      <c r="D156" s="1">
+        <v>4.6331071499999998</v>
+      </c>
+      <c r="E156" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F156">
+        <v>50</v>
+      </c>
+      <c r="G156">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>2</v>
+      </c>
+      <c r="B157">
+        <v>6</v>
+      </c>
+      <c r="C157" s="1">
+        <v>30.941666666666698</v>
+      </c>
+      <c r="D157" s="1">
+        <v>12.5605051</v>
+      </c>
+      <c r="E157" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F157">
+        <v>50</v>
+      </c>
+      <c r="G157">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>3</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="C158" s="1">
+        <v>5.4666666666666703</v>
+      </c>
+      <c r="D158" s="1">
+        <v>2.6776289800000002</v>
+      </c>
+      <c r="E158" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F158">
+        <v>50</v>
+      </c>
+      <c r="G158">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>3</v>
+      </c>
+      <c r="B159">
+        <v>2</v>
+      </c>
+      <c r="C159" s="1">
+        <v>8.9083333333333297</v>
+      </c>
+      <c r="D159" s="1">
+        <v>3.2814792499999998</v>
+      </c>
+      <c r="E159" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F159">
+        <v>50</v>
+      </c>
+      <c r="G159">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>3</v>
+      </c>
+      <c r="B160">
+        <v>3</v>
+      </c>
+      <c r="C160" s="1">
+        <v>21.975000000000001</v>
+      </c>
+      <c r="D160" s="1">
+        <v>9.1335669599999996</v>
+      </c>
+      <c r="E160" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F160">
+        <v>50</v>
+      </c>
+      <c r="G160">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>3</v>
+      </c>
+      <c r="B161">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1">
+        <v>6.0916666666666703</v>
+      </c>
+      <c r="D161" s="1">
+        <v>2.81633493</v>
+      </c>
+      <c r="E161" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F161">
+        <v>50</v>
+      </c>
+      <c r="G161">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>3</v>
+      </c>
+      <c r="B162">
+        <v>5</v>
+      </c>
+      <c r="C162" s="1">
+        <v>9.2750000000000004</v>
+      </c>
+      <c r="D162" s="1">
+        <v>3.4892367000000002</v>
+      </c>
+      <c r="E162" s="2">
+        <v>44796</v>
+      </c>
+      <c r="F162">
+        <v>50</v>
+      </c>
+      <c r="G162">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>3</v>
+      </c>
+      <c r="B163">
+        <v>6</v>
+      </c>
+      <c r="C163" s="1">
         <v>14.783333333333299</v>
       </c>
-      <c r="D145" s="1">
+      <c r="D163" s="1">
         <v>7.5559529000000003</v>
       </c>
-      <c r="E145" s="2">
+      <c r="E163" s="2">
         <v>44796</v>
       </c>
-      <c r="F145">
+      <c r="F163">
         <v>50</v>
       </c>
-      <c r="G145">
+      <c r="G163">
         <v>591</v>
       </c>
     </row>

</xml_diff>